<commit_message>
added some new results
</commit_message>
<xml_diff>
--- a/results/combinedresults/dqbf19.xlsx
+++ b/results/combinedresults/dqbf19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jurajsic/OneDrive/skola/magisterFI/diplomka/DQBFbenchmarks/results/combinedresults/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C1CEBB-ED16-DE45-A3CA-7AF378BFBE52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87DE2CE-7A89-6F47-BE8C-1FDFF056F70A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15360" activeTab="2" xr2:uid="{5DD0E6D6-7882-E44F-A577-7B002FAE22A9}"/>
   </bookViews>
@@ -21436,8 +21436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{130FAACC-10E2-5C4D-978B-741FB3F1F2DB}">
   <dimension ref="A1:Q251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A230" workbookViewId="0">
-      <selection activeCell="L257" sqref="L257"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated some stuff, added new version of DQBDD
</commit_message>
<xml_diff>
--- a/results/combinedresults/dqbf19.xlsx
+++ b/results/combinedresults/dqbf19.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jurajsic/OneDrive/skola/magisterFI/diplomka/DQBFbenchmarks/results/combinedresults/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A73CCA-8378-C14A-9159-C5C486F75AA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8D53FE-FA69-3A40-B78B-216275AB740F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15360" activeTab="1" xr2:uid="{5DD0E6D6-7882-E44F-A577-7B002FAE22A9}"/>
+    <workbookView xWindow="780" yWindow="940" windowWidth="27640" windowHeight="15360" activeTab="1" xr2:uid="{5DD0E6D6-7882-E44F-A577-7B002FAE22A9}"/>
   </bookViews>
   <sheets>
     <sheet name="runs" sheetId="1" r:id="rId1"/>
     <sheet name="realtime" sheetId="2" r:id="rId2"/>
     <sheet name="dqbdd" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">dqbdd!$A$1:$Q$251</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">realtime!$A$1:$M$252</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4334" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4587" uniqueCount="278">
   <si>
     <t>tool</t>
   </si>
@@ -867,6 +871,9 @@
   <si>
     <t>dCAQE 4.0.1</t>
   </si>
+  <si>
+    <t>uniquely solved (this is wrong, needs to remove DQBDD tree)</t>
+  </si>
 </sst>
 </file>
 
@@ -18185,10 +18192,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E88B51B-86D8-E547-9986-F518581AF70F}">
-  <dimension ref="A1:K251"/>
+  <dimension ref="A1:M252"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E255" sqref="E255"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="F253" sqref="F253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18199,9 +18206,11 @@
     <col min="4" max="5" width="19.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -18235,8 +18244,14 @@
       <c r="K1" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" t="s">
+        <v>269</v>
+      </c>
+      <c r="M1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -18270,8 +18285,14 @@
       <c r="K2" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2" t="s">
+        <v>270</v>
+      </c>
+      <c r="M2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -18305,8 +18326,14 @@
       <c r="K3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -18343,8 +18370,14 @@
       <c r="K4">
         <v>901.64800969700002</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4" t="s">
+        <v>260</v>
+      </c>
+      <c r="M4">
+        <v>901.68670359700002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -18381,8 +18414,14 @@
       <c r="K5">
         <v>901.77224028299997</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5" t="s">
+        <v>260</v>
+      </c>
+      <c r="M5">
+        <v>901.90349689799996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -18419,8 +18458,14 @@
       <c r="K6">
         <v>901.74168997300001</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6" t="s">
+        <v>260</v>
+      </c>
+      <c r="M6">
+        <v>901.79542871900003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -18457,8 +18502,14 @@
       <c r="K7">
         <v>901.77521545800005</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7" t="s">
+        <v>260</v>
+      </c>
+      <c r="M7">
+        <v>901.89486329900001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -18495,8 +18546,14 @@
       <c r="K8">
         <v>901.75694320699995</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8" t="s">
+        <v>260</v>
+      </c>
+      <c r="M8">
+        <v>901.81605079200006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -18533,8 +18590,14 @@
       <c r="K9">
         <v>700.28489393899997</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9" t="s">
+        <v>261</v>
+      </c>
+      <c r="M9">
+        <v>421.68146624600001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -18571,8 +18634,14 @@
       <c r="K10">
         <v>0.70292877600000003</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10" t="s">
+        <v>258</v>
+      </c>
+      <c r="M10">
+        <v>0.45031598499999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -18609,8 +18678,14 @@
       <c r="K11">
         <v>0.35866247299999998</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11" t="s">
+        <v>258</v>
+      </c>
+      <c r="M11">
+        <v>0.47832879</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -18647,8 +18722,14 @@
       <c r="K12">
         <v>36.429104823000003</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12" t="s">
+        <v>258</v>
+      </c>
+      <c r="M12">
+        <v>23.979405363000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -18685,8 +18766,14 @@
       <c r="K13">
         <v>35.307914566999997</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13" t="s">
+        <v>260</v>
+      </c>
+      <c r="M13">
+        <v>901.74665096599995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -18723,8 +18810,14 @@
       <c r="K14">
         <v>0.106500795</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14" t="s">
+        <v>258</v>
+      </c>
+      <c r="M14">
+        <v>9.5362682000000004E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -18761,8 +18854,14 @@
       <c r="K15">
         <v>0.17856962000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15" t="s">
+        <v>258</v>
+      </c>
+      <c r="M15">
+        <v>0.17877522900000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -18799,8 +18898,14 @@
       <c r="K16">
         <v>92.006030260000003</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16" t="s">
+        <v>261</v>
+      </c>
+      <c r="M16">
+        <v>92.409753330000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -18837,8 +18942,14 @@
       <c r="K17">
         <v>92.989088621999997</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17" t="s">
+        <v>261</v>
+      </c>
+      <c r="M17">
+        <v>93.809883024000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -18875,8 +18986,14 @@
       <c r="K18">
         <v>92.084711827999996</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18" t="s">
+        <v>261</v>
+      </c>
+      <c r="M18">
+        <v>91.721492924000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -18913,8 +19030,14 @@
       <c r="K19">
         <v>91.618017336999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19" t="s">
+        <v>261</v>
+      </c>
+      <c r="M19">
+        <v>91.176365832000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -18951,8 +19074,14 @@
       <c r="K20">
         <v>91.741512951999994</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20" t="s">
+        <v>261</v>
+      </c>
+      <c r="M20">
+        <v>90.853693308000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -18989,8 +19118,14 @@
       <c r="K21">
         <v>91.543883679999993</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21" t="s">
+        <v>261</v>
+      </c>
+      <c r="M21">
+        <v>91.237849724</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -19027,8 +19162,14 @@
       <c r="K22">
         <v>91.166503066999994</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L22" t="s">
+        <v>261</v>
+      </c>
+      <c r="M22">
+        <v>91.784116010000005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -19065,8 +19206,14 @@
       <c r="K23">
         <v>91.154769763000004</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23" t="s">
+        <v>261</v>
+      </c>
+      <c r="M23">
+        <v>90.638299919999994</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -19103,8 +19250,14 @@
       <c r="K24">
         <v>91.826081650999996</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L24" t="s">
+        <v>261</v>
+      </c>
+      <c r="M24">
+        <v>91.654322741000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -19141,8 +19294,14 @@
       <c r="K25">
         <v>91.700815677999998</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L25" t="s">
+        <v>261</v>
+      </c>
+      <c r="M25">
+        <v>91.592912287999994</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -19179,8 +19338,14 @@
       <c r="K26">
         <v>92.430378481000005</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L26" t="s">
+        <v>261</v>
+      </c>
+      <c r="M26">
+        <v>90.888190644000005</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -19217,8 +19382,14 @@
       <c r="K27">
         <v>91.852101795999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L27" t="s">
+        <v>261</v>
+      </c>
+      <c r="M27">
+        <v>91.985865378</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -19255,8 +19426,14 @@
       <c r="K28">
         <v>92.238658811999997</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L28" t="s">
+        <v>261</v>
+      </c>
+      <c r="M28">
+        <v>91.534013588999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -19293,8 +19470,14 @@
       <c r="K29">
         <v>92.366042504999996</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L29" t="s">
+        <v>261</v>
+      </c>
+      <c r="M29">
+        <v>92.075464421000007</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -19331,8 +19514,14 @@
       <c r="K30">
         <v>91.59423323</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L30" t="s">
+        <v>261</v>
+      </c>
+      <c r="M30">
+        <v>92.121324090000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -19369,8 +19558,14 @@
       <c r="K31">
         <v>199.18659537299999</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L31" t="s">
+        <v>261</v>
+      </c>
+      <c r="M31">
+        <v>202.88463577600001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -19407,8 +19602,14 @@
       <c r="K32">
         <v>901.76950887099997</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L32" t="s">
+        <v>261</v>
+      </c>
+      <c r="M32">
+        <v>165.697857863</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -19445,8 +19646,14 @@
       <c r="K33">
         <v>901.64950479499998</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L33" t="s">
+        <v>261</v>
+      </c>
+      <c r="M33">
+        <v>167.18481085499999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -19483,8 +19690,14 @@
       <c r="K34">
         <v>104.795602454</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L34" t="s">
+        <v>261</v>
+      </c>
+      <c r="M34">
+        <v>103.07008250299999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -19521,8 +19734,14 @@
       <c r="K35">
         <v>0.17829984500000001</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L35" t="s">
+        <v>258</v>
+      </c>
+      <c r="M35">
+        <v>0.161592448</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -19559,8 +19778,14 @@
       <c r="K36">
         <v>118.527558399</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L36" t="s">
+        <v>261</v>
+      </c>
+      <c r="M36">
+        <v>82.790511073000005</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -19597,8 +19822,14 @@
       <c r="K37">
         <v>119.502452451</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L37" t="s">
+        <v>261</v>
+      </c>
+      <c r="M37">
+        <v>82.025603649000004</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -19635,8 +19866,14 @@
       <c r="K38">
         <v>2.2334657000000001E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L38" t="s">
+        <v>258</v>
+      </c>
+      <c r="M38">
+        <v>2.1929276000000001E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -19673,8 +19910,14 @@
       <c r="K39">
         <v>4.2451867999999997E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L39" t="s">
+        <v>258</v>
+      </c>
+      <c r="M39">
+        <v>0.137990378</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -19711,8 +19954,14 @@
       <c r="K40">
         <v>4.2462120999999999E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L40" t="s">
+        <v>258</v>
+      </c>
+      <c r="M40">
+        <v>0.13767146299999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -19749,8 +19998,14 @@
       <c r="K41">
         <v>6.2501161999999999E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L41" t="s">
+        <v>260</v>
+      </c>
+      <c r="M41">
+        <v>901.56078541399995</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -19787,8 +20042,14 @@
       <c r="K42">
         <v>1.2111820799999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L42" t="s">
+        <v>258</v>
+      </c>
+      <c r="M42">
+        <v>0.67040133700000004</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -19825,8 +20086,14 @@
       <c r="K43">
         <v>94.167303046000001</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L43" t="s">
+        <v>261</v>
+      </c>
+      <c r="M43">
+        <v>93.938432625000004</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>50</v>
       </c>
@@ -19863,8 +20130,14 @@
       <c r="K44">
         <v>93.470529346000006</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L44" t="s">
+        <v>261</v>
+      </c>
+      <c r="M44">
+        <v>90.971360128000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>51</v>
       </c>
@@ -19901,8 +20174,14 @@
       <c r="K45">
         <v>93.930470037999996</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L45" t="s">
+        <v>261</v>
+      </c>
+      <c r="M45">
+        <v>91.344669027999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -19939,8 +20218,14 @@
       <c r="K46">
         <v>94.351260838000002</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L46" t="s">
+        <v>261</v>
+      </c>
+      <c r="M46">
+        <v>91.160639545999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>53</v>
       </c>
@@ -19977,8 +20262,14 @@
       <c r="K47">
         <v>93.415116585000007</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L47" t="s">
+        <v>261</v>
+      </c>
+      <c r="M47">
+        <v>93.906236213</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>54</v>
       </c>
@@ -20015,8 +20306,14 @@
       <c r="K48">
         <v>94.425819880999995</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L48" t="s">
+        <v>261</v>
+      </c>
+      <c r="M48">
+        <v>91.475795821999995</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -20053,8 +20350,14 @@
       <c r="K49">
         <v>94.807211766999998</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L49" t="s">
+        <v>261</v>
+      </c>
+      <c r="M49">
+        <v>91.791674111000006</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -20091,8 +20394,14 @@
       <c r="K50">
         <v>95.684294347999995</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L50" t="s">
+        <v>261</v>
+      </c>
+      <c r="M50">
+        <v>93.879619138999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>57</v>
       </c>
@@ -20129,8 +20438,14 @@
       <c r="K51">
         <v>94.607935365000003</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L51" t="s">
+        <v>261</v>
+      </c>
+      <c r="M51">
+        <v>90.636046754999995</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -20167,8 +20482,14 @@
       <c r="K52">
         <v>93.666824465999994</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L52" t="s">
+        <v>261</v>
+      </c>
+      <c r="M52">
+        <v>94.194321392999996</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -20205,8 +20526,14 @@
       <c r="K53">
         <v>93.930237903000005</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L53" t="s">
+        <v>261</v>
+      </c>
+      <c r="M53">
+        <v>91.278266833999993</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>60</v>
       </c>
@@ -20243,8 +20570,14 @@
       <c r="K54">
         <v>94.663555833000004</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L54" t="s">
+        <v>261</v>
+      </c>
+      <c r="M54">
+        <v>91.701483087</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>61</v>
       </c>
@@ -20281,8 +20614,14 @@
       <c r="K55">
         <v>94.059656641999993</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L55" t="s">
+        <v>261</v>
+      </c>
+      <c r="M55">
+        <v>90.979492633000007</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>62</v>
       </c>
@@ -20319,8 +20658,14 @@
       <c r="K56">
         <v>94.235041957000007</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L56" t="s">
+        <v>261</v>
+      </c>
+      <c r="M56">
+        <v>93.137301840999996</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -20357,8 +20702,14 @@
       <c r="K57">
         <v>94.595820587000006</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L57" t="s">
+        <v>261</v>
+      </c>
+      <c r="M57">
+        <v>92.193087313999996</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>64</v>
       </c>
@@ -20395,8 +20746,14 @@
       <c r="K58">
         <v>94.851754502999995</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L58" t="s">
+        <v>261</v>
+      </c>
+      <c r="M58">
+        <v>91.031792881000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>65</v>
       </c>
@@ -20433,8 +20790,14 @@
       <c r="K59">
         <v>94.211636345000002</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L59" t="s">
+        <v>261</v>
+      </c>
+      <c r="M59">
+        <v>91.584884463999998</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -20471,8 +20834,14 @@
       <c r="K60">
         <v>94.383133607999994</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L60" t="s">
+        <v>261</v>
+      </c>
+      <c r="M60">
+        <v>92.017093083999995</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>67</v>
       </c>
@@ -20509,8 +20878,14 @@
       <c r="K61">
         <v>95.05607277</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L61" t="s">
+        <v>261</v>
+      </c>
+      <c r="M61">
+        <v>92.826517652000007</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>68</v>
       </c>
@@ -20547,8 +20922,14 @@
       <c r="K62">
         <v>95.119855356000002</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L62" t="s">
+        <v>261</v>
+      </c>
+      <c r="M62">
+        <v>92.103174640000006</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>69</v>
       </c>
@@ -20585,8 +20966,14 @@
       <c r="K63">
         <v>230.93735746300001</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L63" t="s">
+        <v>261</v>
+      </c>
+      <c r="M63">
+        <v>113.311629457</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>70</v>
       </c>
@@ -20623,8 +21010,14 @@
       <c r="K64">
         <v>604.41194019099999</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L64" t="s">
+        <v>261</v>
+      </c>
+      <c r="M64">
+        <v>92.565266691999994</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>71</v>
       </c>
@@ -20661,8 +21054,14 @@
       <c r="K65">
         <v>156.22454471500001</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L65" t="s">
+        <v>261</v>
+      </c>
+      <c r="M65">
+        <v>154.59128110200001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>72</v>
       </c>
@@ -20699,8 +21098,14 @@
       <c r="K66">
         <v>99.855296870999993</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L66" t="s">
+        <v>261</v>
+      </c>
+      <c r="M66">
+        <v>95.985286135999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>73</v>
       </c>
@@ -20737,8 +21142,14 @@
       <c r="K67">
         <v>98.690210441000005</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L67" t="s">
+        <v>261</v>
+      </c>
+      <c r="M67">
+        <v>95.700674887999995</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>74</v>
       </c>
@@ -20775,8 +21186,14 @@
       <c r="K68">
         <v>93.327115926000005</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L68" t="s">
+        <v>261</v>
+      </c>
+      <c r="M68">
+        <v>90.772248934000004</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>75</v>
       </c>
@@ -20813,8 +21230,14 @@
       <c r="K69">
         <v>93.447009187000006</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L69" t="s">
+        <v>261</v>
+      </c>
+      <c r="M69">
+        <v>92.201844096000002</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>76</v>
       </c>
@@ -20851,8 +21274,14 @@
       <c r="K70">
         <v>92.790100271</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L70" t="s">
+        <v>261</v>
+      </c>
+      <c r="M70">
+        <v>90.726496840999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>77</v>
       </c>
@@ -20889,8 +21318,14 @@
       <c r="K71">
         <v>92.338273220999994</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L71" t="s">
+        <v>261</v>
+      </c>
+      <c r="M71">
+        <v>92.466103903999993</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>78</v>
       </c>
@@ -20927,8 +21362,14 @@
       <c r="K72">
         <v>91.917602469000002</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L72" t="s">
+        <v>261</v>
+      </c>
+      <c r="M72">
+        <v>91.160605329999996</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>79</v>
       </c>
@@ -20965,8 +21406,14 @@
       <c r="K73">
         <v>91.257697049000001</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L73" t="s">
+        <v>261</v>
+      </c>
+      <c r="M73">
+        <v>90.902817323999997</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>80</v>
       </c>
@@ -21003,8 +21450,14 @@
       <c r="K74">
         <v>91.433949646000002</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L74" t="s">
+        <v>261</v>
+      </c>
+      <c r="M74">
+        <v>92.525009983999993</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>81</v>
       </c>
@@ -21041,8 +21494,14 @@
       <c r="K75">
         <v>92.737290024000004</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L75" t="s">
+        <v>261</v>
+      </c>
+      <c r="M75">
+        <v>91.462876562999995</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>82</v>
       </c>
@@ -21079,8 +21538,14 @@
       <c r="K76">
         <v>92.410392852000001</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L76" t="s">
+        <v>261</v>
+      </c>
+      <c r="M76">
+        <v>92.025858726999999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>83</v>
       </c>
@@ -21117,8 +21582,14 @@
       <c r="K77">
         <v>91.865507132999994</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L77" t="s">
+        <v>261</v>
+      </c>
+      <c r="M77">
+        <v>91.247291001999997</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>84</v>
       </c>
@@ -21155,8 +21626,14 @@
       <c r="K78">
         <v>91.529879629000007</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L78" t="s">
+        <v>261</v>
+      </c>
+      <c r="M78">
+        <v>91.026988492000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>85</v>
       </c>
@@ -21193,8 +21670,14 @@
       <c r="K79">
         <v>91.725563831000002</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L79" t="s">
+        <v>261</v>
+      </c>
+      <c r="M79">
+        <v>93.426645770999997</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>86</v>
       </c>
@@ -21231,8 +21714,14 @@
       <c r="K80">
         <v>94.304636857999995</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L80" t="s">
+        <v>261</v>
+      </c>
+      <c r="M80">
+        <v>92.640763108000002</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>87</v>
       </c>
@@ -21269,8 +21758,14 @@
       <c r="K81">
         <v>48.017604024999997</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L81" t="s">
+        <v>258</v>
+      </c>
+      <c r="M81">
+        <v>317.95066357600001</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>88</v>
       </c>
@@ -21307,8 +21802,14 @@
       <c r="K82">
         <v>30.214337549</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L82" t="s">
+        <v>261</v>
+      </c>
+      <c r="M82">
+        <v>102.672164391</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>89</v>
       </c>
@@ -21345,8 +21846,14 @@
       <c r="K83">
         <v>34.691493741000002</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L83" t="s">
+        <v>261</v>
+      </c>
+      <c r="M83">
+        <v>96.000258054</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>90</v>
       </c>
@@ -21383,8 +21890,14 @@
       <c r="K84">
         <v>3.4096346E-2</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L84" t="s">
+        <v>258</v>
+      </c>
+      <c r="M84">
+        <v>3.3530022E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>91</v>
       </c>
@@ -21421,8 +21934,14 @@
       <c r="K85">
         <v>1.3392598790000001</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L85" t="s">
+        <v>258</v>
+      </c>
+      <c r="M85">
+        <v>14.500450731999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>92</v>
       </c>
@@ -21459,8 +21978,14 @@
       <c r="K86">
         <v>30.976314704</v>
       </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L86" t="s">
+        <v>261</v>
+      </c>
+      <c r="M86">
+        <v>184.11971844000001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>93</v>
       </c>
@@ -21497,8 +22022,14 @@
       <c r="K87">
         <v>46.315922520000001</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L87" t="s">
+        <v>258</v>
+      </c>
+      <c r="M87">
+        <v>2.5819676999999999E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>94</v>
       </c>
@@ -21535,8 +22066,14 @@
       <c r="K88">
         <v>24.372071473999998</v>
       </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L88" t="s">
+        <v>261</v>
+      </c>
+      <c r="M88">
+        <v>81.877951225999993</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>95</v>
       </c>
@@ -21573,8 +22110,14 @@
       <c r="K89">
         <v>25.183163863000001</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L89" t="s">
+        <v>261</v>
+      </c>
+      <c r="M89">
+        <v>144.163868511</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>96</v>
       </c>
@@ -21611,8 +22154,14 @@
       <c r="K90">
         <v>6.2146934000000001E-2</v>
       </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L90" t="s">
+        <v>258</v>
+      </c>
+      <c r="M90">
+        <v>0.598268727</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>97</v>
       </c>
@@ -21649,8 +22198,14 @@
       <c r="K91">
         <v>5.821759E-2</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L91" t="s">
+        <v>258</v>
+      </c>
+      <c r="M91">
+        <v>0.58231676499999996</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>98</v>
       </c>
@@ -21687,8 +22242,14 @@
       <c r="K92">
         <v>182.888385363</v>
       </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L92" t="s">
+        <v>261</v>
+      </c>
+      <c r="M92">
+        <v>52.752273367000001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>99</v>
       </c>
@@ -21725,8 +22286,14 @@
       <c r="K93">
         <v>901.67362746499998</v>
       </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L93" t="s">
+        <v>261</v>
+      </c>
+      <c r="M93">
+        <v>721.47601106000002</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>100</v>
       </c>
@@ -21763,8 +22330,14 @@
       <c r="K94">
         <v>901.80022778299997</v>
       </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L94" t="s">
+        <v>261</v>
+      </c>
+      <c r="M94">
+        <v>895.03549405399997</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>101</v>
       </c>
@@ -21801,8 +22374,14 @@
       <c r="K95">
         <v>901.76958070700005</v>
       </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L95" t="s">
+        <v>260</v>
+      </c>
+      <c r="M95">
+        <v>901.86282717799997</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>102</v>
       </c>
@@ -21839,8 +22418,14 @@
       <c r="K96">
         <v>392.54938571999998</v>
       </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L96" t="s">
+        <v>260</v>
+      </c>
+      <c r="M96">
+        <v>901.85668597999995</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>103</v>
       </c>
@@ -21877,8 +22462,14 @@
       <c r="K97">
         <v>83.058983788999996</v>
       </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L97" t="s">
+        <v>260</v>
+      </c>
+      <c r="M97">
+        <v>901.70146854999996</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>104</v>
       </c>
@@ -21915,8 +22506,14 @@
       <c r="K98">
         <v>3.2564652249999999</v>
       </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L98" t="s">
+        <v>260</v>
+      </c>
+      <c r="M98">
+        <v>901.75112388699995</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>105</v>
       </c>
@@ -21953,8 +22550,14 @@
       <c r="K99">
         <v>285.13016284100001</v>
       </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L99" t="s">
+        <v>261</v>
+      </c>
+      <c r="M99">
+        <v>285.64037744199999</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>106</v>
       </c>
@@ -21991,8 +22594,14 @@
       <c r="K100">
         <v>2.828258623</v>
       </c>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L100" t="s">
+        <v>258</v>
+      </c>
+      <c r="M100">
+        <v>0.101749882</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>107</v>
       </c>
@@ -22029,8 +22638,14 @@
       <c r="K101">
         <v>329.04456174799998</v>
       </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L101" t="s">
+        <v>261</v>
+      </c>
+      <c r="M101">
+        <v>289.01687954900001</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>108</v>
       </c>
@@ -22067,8 +22682,14 @@
       <c r="K102">
         <v>0.13428179000000001</v>
       </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L102" t="s">
+        <v>259</v>
+      </c>
+      <c r="M102">
+        <v>0.12996542699999999</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>109</v>
       </c>
@@ -22105,8 +22726,14 @@
       <c r="K103">
         <v>2.2679092729999999</v>
       </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L103" t="s">
+        <v>260</v>
+      </c>
+      <c r="M103">
+        <v>901.73639270800004</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>110</v>
       </c>
@@ -22143,8 +22770,14 @@
       <c r="K104">
         <v>1.831670669</v>
       </c>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L104" t="s">
+        <v>260</v>
+      </c>
+      <c r="M104">
+        <v>901.80911093600002</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>111</v>
       </c>
@@ -22181,8 +22814,14 @@
       <c r="K105">
         <v>312.56458874999998</v>
       </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L105" t="s">
+        <v>261</v>
+      </c>
+      <c r="M105">
+        <v>758.21690201199999</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>112</v>
       </c>
@@ -22219,8 +22858,14 @@
       <c r="K106">
         <v>290.33830643700003</v>
       </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L106" t="s">
+        <v>261</v>
+      </c>
+      <c r="M106">
+        <v>312.19893248699998</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>113</v>
       </c>
@@ -22257,8 +22902,14 @@
       <c r="K107">
         <v>252.91615484299999</v>
       </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L107" t="s">
+        <v>261</v>
+      </c>
+      <c r="M107">
+        <v>288.24064765700001</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>114</v>
       </c>
@@ -22295,8 +22946,14 @@
       <c r="K108">
         <v>0.19839812100000001</v>
       </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L108" t="s">
+        <v>259</v>
+      </c>
+      <c r="M108">
+        <v>0.19384426900000001</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>115</v>
       </c>
@@ -22333,8 +22990,14 @@
       <c r="K109">
         <v>0.162484824</v>
       </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L109" t="s">
+        <v>259</v>
+      </c>
+      <c r="M109">
+        <v>0.16197946899999999</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>116</v>
       </c>
@@ -22371,8 +23034,14 @@
       <c r="K110">
         <v>266.50600411200003</v>
       </c>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L110" t="s">
+        <v>261</v>
+      </c>
+      <c r="M110">
+        <v>681.80943971900001</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>117</v>
       </c>
@@ -22409,8 +23078,14 @@
       <c r="K111">
         <v>218.564592847</v>
       </c>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L111" t="s">
+        <v>261</v>
+      </c>
+      <c r="M111">
+        <v>264.52458167600003</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>118</v>
       </c>
@@ -22447,8 +23122,14 @@
       <c r="K112">
         <v>8.3644410750000002</v>
       </c>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L112" t="s">
+        <v>258</v>
+      </c>
+      <c r="M112">
+        <v>68.396624497999994</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>119</v>
       </c>
@@ -22485,8 +23166,14 @@
       <c r="K113">
         <v>8.7607907380000007</v>
       </c>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L113" t="s">
+        <v>259</v>
+      </c>
+      <c r="M113">
+        <v>119.12664254400001</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>120</v>
       </c>
@@ -22523,8 +23210,14 @@
       <c r="K114">
         <v>11.09830112</v>
       </c>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L114" t="s">
+        <v>259</v>
+      </c>
+      <c r="M114">
+        <v>22.282320501000001</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>121</v>
       </c>
@@ -22561,8 +23254,14 @@
       <c r="K115">
         <v>8.3363819479999997</v>
       </c>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L115" t="s">
+        <v>259</v>
+      </c>
+      <c r="M115">
+        <v>62.852743189000002</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>122</v>
       </c>
@@ -22599,8 +23298,14 @@
       <c r="K116">
         <v>18.567895797999999</v>
       </c>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L116" t="s">
+        <v>258</v>
+      </c>
+      <c r="M116">
+        <v>749.87047708700004</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>123</v>
       </c>
@@ -22637,8 +23342,14 @@
       <c r="K117">
         <v>10.125471866</v>
       </c>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L117" t="s">
+        <v>260</v>
+      </c>
+      <c r="M117">
+        <v>901.727393076</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>124</v>
       </c>
@@ -22675,8 +23386,14 @@
       <c r="K118">
         <v>0.362512377</v>
       </c>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L118" t="s">
+        <v>258</v>
+      </c>
+      <c r="M118">
+        <v>6.0374380810000003</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>125</v>
       </c>
@@ -22713,8 +23430,14 @@
       <c r="K119">
         <v>4.013287482</v>
       </c>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L119" t="s">
+        <v>259</v>
+      </c>
+      <c r="M119">
+        <v>9.5843368089999998</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>126</v>
       </c>
@@ -22751,8 +23474,14 @@
       <c r="K120">
         <v>0.21000259199999999</v>
       </c>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L120" t="s">
+        <v>259</v>
+      </c>
+      <c r="M120">
+        <v>8.3666505010000005</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>127</v>
       </c>
@@ -22789,8 +23518,14 @@
       <c r="K121">
         <v>5.750423316</v>
       </c>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L121" t="s">
+        <v>259</v>
+      </c>
+      <c r="M121">
+        <v>4.2081603750000003</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>128</v>
       </c>
@@ -22827,8 +23562,14 @@
       <c r="K122">
         <v>0.246462708</v>
       </c>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L122" t="s">
+        <v>258</v>
+      </c>
+      <c r="M122">
+        <v>8.2588015119999998</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>129</v>
       </c>
@@ -22865,8 +23606,14 @@
       <c r="K123">
         <v>4.8658859449999996</v>
       </c>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L123" t="s">
+        <v>259</v>
+      </c>
+      <c r="M123">
+        <v>2.234756285</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>130</v>
       </c>
@@ -22903,8 +23650,14 @@
       <c r="K124">
         <v>110.63426251200001</v>
       </c>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L124" t="s">
+        <v>261</v>
+      </c>
+      <c r="M124">
+        <v>126.841352896</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>131</v>
       </c>
@@ -22941,8 +23694,14 @@
       <c r="K125">
         <v>0.19820307000000001</v>
       </c>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L125" t="s">
+        <v>259</v>
+      </c>
+      <c r="M125">
+        <v>3.37590557</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>132</v>
       </c>
@@ -22979,8 +23738,14 @@
       <c r="K126">
         <v>4.9526476190000004</v>
       </c>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L126" t="s">
+        <v>259</v>
+      </c>
+      <c r="M126">
+        <v>2.219374111</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>133</v>
       </c>
@@ -23017,8 +23782,14 @@
       <c r="K127">
         <v>1.1069611109999999</v>
       </c>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L127" t="s">
+        <v>258</v>
+      </c>
+      <c r="M127">
+        <v>0.73418394099999995</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>134</v>
       </c>
@@ -23055,8 +23826,14 @@
       <c r="K128">
         <v>1.3919023079999999</v>
       </c>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L128" t="s">
+        <v>259</v>
+      </c>
+      <c r="M128">
+        <v>0.77841205099999999</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>135</v>
       </c>
@@ -23093,8 +23870,14 @@
       <c r="K129">
         <v>1.603363852</v>
       </c>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L129" t="s">
+        <v>258</v>
+      </c>
+      <c r="M129">
+        <v>0.69441493300000001</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>136</v>
       </c>
@@ -23131,8 +23914,14 @@
       <c r="K130">
         <v>1.751915879</v>
       </c>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L130" t="s">
+        <v>259</v>
+      </c>
+      <c r="M130">
+        <v>0.95457138500000005</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>137</v>
       </c>
@@ -23169,8 +23958,14 @@
       <c r="K131">
         <v>1.5959490649999999</v>
       </c>
-    </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L131" t="s">
+        <v>259</v>
+      </c>
+      <c r="M131">
+        <v>0.67042240600000003</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>138</v>
       </c>
@@ -23207,8 +24002,14 @@
       <c r="K132">
         <v>2.0797560609999999</v>
       </c>
-    </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L132" t="s">
+        <v>259</v>
+      </c>
+      <c r="M132">
+        <v>2.227327898</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>139</v>
       </c>
@@ -23245,8 +24046,14 @@
       <c r="K133">
         <v>2.1322692860000001</v>
       </c>
-    </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L133" t="s">
+        <v>259</v>
+      </c>
+      <c r="M133">
+        <v>3.8963631400000001</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>140</v>
       </c>
@@ -23283,8 +24090,14 @@
       <c r="K134">
         <v>1.879507155</v>
       </c>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L134" t="s">
+        <v>259</v>
+      </c>
+      <c r="M134">
+        <v>2.471347593</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>141</v>
       </c>
@@ -23321,8 +24134,14 @@
       <c r="K135">
         <v>3.268631638</v>
       </c>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L135" t="s">
+        <v>261</v>
+      </c>
+      <c r="M135">
+        <v>240.38835290700001</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>142</v>
       </c>
@@ -23359,8 +24178,14 @@
       <c r="K136">
         <v>0.56745813300000003</v>
       </c>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L136" t="s">
+        <v>259</v>
+      </c>
+      <c r="M136">
+        <v>483.20236474199999</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>143</v>
       </c>
@@ -23397,8 +24222,14 @@
       <c r="K137">
         <v>3.4285483960000001</v>
       </c>
-    </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L137" t="s">
+        <v>261</v>
+      </c>
+      <c r="M137">
+        <v>218.622913168</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>144</v>
       </c>
@@ -23435,8 +24266,14 @@
       <c r="K138">
         <v>2.6603280570000001</v>
       </c>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L138" t="s">
+        <v>260</v>
+      </c>
+      <c r="M138">
+        <v>901.60462567900004</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>145</v>
       </c>
@@ -23473,8 +24310,14 @@
       <c r="K139">
         <v>2.0478815400000001</v>
       </c>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L139" t="s">
+        <v>258</v>
+      </c>
+      <c r="M139">
+        <v>4.5328894550000003</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>146</v>
       </c>
@@ -23511,8 +24354,14 @@
       <c r="K140">
         <v>7.499741738</v>
       </c>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L140" t="s">
+        <v>259</v>
+      </c>
+      <c r="M140">
+        <v>4.7089380409999997</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>147</v>
       </c>
@@ -23549,8 +24398,14 @@
       <c r="K141">
         <v>1.920552139</v>
       </c>
-    </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L141" t="s">
+        <v>258</v>
+      </c>
+      <c r="M141">
+        <v>1.998844163</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>148</v>
       </c>
@@ -23587,8 +24442,14 @@
       <c r="K142">
         <v>0.27086375800000001</v>
       </c>
-    </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L142" t="s">
+        <v>259</v>
+      </c>
+      <c r="M142">
+        <v>416.90210300699999</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>149</v>
       </c>
@@ -23625,8 +24486,14 @@
       <c r="K143">
         <v>7.0312686999999999E-2</v>
       </c>
-    </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L143" t="s">
+        <v>259</v>
+      </c>
+      <c r="M143">
+        <v>6.9754878000000006E-2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>150</v>
       </c>
@@ -23663,8 +24530,14 @@
       <c r="K144">
         <v>378.321390538</v>
       </c>
-    </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L144" t="s">
+        <v>260</v>
+      </c>
+      <c r="M144">
+        <v>901.72192235</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>151</v>
       </c>
@@ -23701,8 +24574,14 @@
       <c r="K145">
         <v>901.64751744600005</v>
       </c>
-    </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L145" t="s">
+        <v>260</v>
+      </c>
+      <c r="M145">
+        <v>901.70730279999998</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>152</v>
       </c>
@@ -23739,8 +24618,14 @@
       <c r="K146">
         <v>870.416823196</v>
       </c>
-    </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L146" t="s">
+        <v>260</v>
+      </c>
+      <c r="M146">
+        <v>901.71131255800003</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>153</v>
       </c>
@@ -23777,8 +24662,14 @@
       <c r="K147">
         <v>383.45581437499999</v>
       </c>
-    </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L147" t="s">
+        <v>260</v>
+      </c>
+      <c r="M147">
+        <v>901.71389984899997</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>154</v>
       </c>
@@ -23815,8 +24706,14 @@
       <c r="K148">
         <v>901.81388293999998</v>
       </c>
-    </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L148" t="s">
+        <v>260</v>
+      </c>
+      <c r="M148">
+        <v>901.70956968600001</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>155</v>
       </c>
@@ -23853,8 +24750,14 @@
       <c r="K149">
         <v>901.75738657199997</v>
       </c>
-    </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L149" t="s">
+        <v>260</v>
+      </c>
+      <c r="M149">
+        <v>901.60518767999997</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>156</v>
       </c>
@@ -23891,8 +24794,14 @@
       <c r="K150">
         <v>901.82434052099995</v>
       </c>
-    </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L150" t="s">
+        <v>260</v>
+      </c>
+      <c r="M150">
+        <v>901.72209818500005</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>157</v>
       </c>
@@ -23929,8 +24838,14 @@
       <c r="K151">
         <v>28.763490174000001</v>
       </c>
-    </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L151" t="s">
+        <v>259</v>
+      </c>
+      <c r="M151">
+        <v>28.806528774</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>158</v>
       </c>
@@ -23967,8 +24882,14 @@
       <c r="K152">
         <v>18.936426086000001</v>
       </c>
-    </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L152" t="s">
+        <v>259</v>
+      </c>
+      <c r="M152">
+        <v>18.907693205000001</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>159</v>
       </c>
@@ -24005,8 +24926,14 @@
       <c r="K153">
         <v>2.4080685019999999</v>
       </c>
-    </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L153" t="s">
+        <v>259</v>
+      </c>
+      <c r="M153">
+        <v>3.7166006989999998</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>160</v>
       </c>
@@ -24043,8 +24970,14 @@
       <c r="K154">
         <v>2.155830243</v>
       </c>
-    </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L154" t="s">
+        <v>259</v>
+      </c>
+      <c r="M154">
+        <v>1.410813675</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>161</v>
       </c>
@@ -24081,8 +25014,14 @@
       <c r="K155">
         <v>18.832949968000001</v>
       </c>
-    </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L155" t="s">
+        <v>259</v>
+      </c>
+      <c r="M155">
+        <v>19.011272508000001</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>162</v>
       </c>
@@ -24119,8 +25058,14 @@
       <c r="K156">
         <v>0.41461776299999997</v>
       </c>
-    </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L156" t="s">
+        <v>258</v>
+      </c>
+      <c r="M156">
+        <v>0.29795597400000001</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>163</v>
       </c>
@@ -24157,8 +25102,14 @@
       <c r="K157">
         <v>1.6714839669999999</v>
       </c>
-    </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L157" t="s">
+        <v>258</v>
+      </c>
+      <c r="M157">
+        <v>1.154659076</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>164</v>
       </c>
@@ -24195,8 +25146,14 @@
       <c r="K158">
         <v>2.151314153</v>
       </c>
-    </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L158" t="s">
+        <v>259</v>
+      </c>
+      <c r="M158">
+        <v>2.7197133519999999</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>165</v>
       </c>
@@ -24233,8 +25190,14 @@
       <c r="K159">
         <v>28.911815976</v>
       </c>
-    </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L159" t="s">
+        <v>258</v>
+      </c>
+      <c r="M159">
+        <v>29.226698196000001</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>166</v>
       </c>
@@ -24271,8 +25234,14 @@
       <c r="K160">
         <v>49.647263721000002</v>
       </c>
-    </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L160" t="s">
+        <v>259</v>
+      </c>
+      <c r="M160">
+        <v>49.710790842999998</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>167</v>
       </c>
@@ -24309,8 +25278,14 @@
       <c r="K161">
         <v>2.1198528599999999</v>
       </c>
-    </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L161" t="s">
+        <v>259</v>
+      </c>
+      <c r="M161">
+        <v>2.711702528</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>168</v>
       </c>
@@ -24347,8 +25322,14 @@
       <c r="K162">
         <v>3.1485379949999999</v>
       </c>
-    </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L162" t="s">
+        <v>259</v>
+      </c>
+      <c r="M162">
+        <v>2.1233887400000002</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>169</v>
       </c>
@@ -24385,8 +25366,14 @@
       <c r="K163">
         <v>28.767696147999999</v>
       </c>
-    </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L163" t="s">
+        <v>259</v>
+      </c>
+      <c r="M163">
+        <v>28.714915801</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>170</v>
       </c>
@@ -24423,8 +25410,14 @@
       <c r="K164">
         <v>0.41017587799999999</v>
       </c>
-    </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L164" t="s">
+        <v>258</v>
+      </c>
+      <c r="M164">
+        <v>0.29394513</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>171</v>
       </c>
@@ -24461,8 +25454,14 @@
       <c r="K165">
         <v>3.8349544999999999E-2</v>
       </c>
-    </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L165" t="s">
+        <v>259</v>
+      </c>
+      <c r="M165">
+        <v>3.3797854000000002E-2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>172</v>
       </c>
@@ -24499,8 +25498,14 @@
       <c r="K166">
         <v>4.6320134999999998E-2</v>
       </c>
-    </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L166" t="s">
+        <v>258</v>
+      </c>
+      <c r="M166">
+        <v>3.7815762000000003E-2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>173</v>
       </c>
@@ -24537,8 +25542,14 @@
       <c r="K167">
         <v>3.8347226999999998E-2</v>
       </c>
-    </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L167" t="s">
+        <v>259</v>
+      </c>
+      <c r="M167">
+        <v>3.3869877999999999E-2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>174</v>
       </c>
@@ -24575,8 +25586,14 @@
       <c r="K168">
         <v>3.8408062999999999E-2</v>
       </c>
-    </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L168" t="s">
+        <v>259</v>
+      </c>
+      <c r="M168">
+        <v>3.3795947E-2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>175</v>
       </c>
@@ -24613,8 +25630,14 @@
       <c r="K169">
         <v>4.6357796E-2</v>
       </c>
-    </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L169" t="s">
+        <v>258</v>
+      </c>
+      <c r="M169">
+        <v>3.7868341E-2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>176</v>
       </c>
@@ -24651,8 +25674,14 @@
       <c r="K170">
         <v>4.6306775000000001E-2</v>
       </c>
-    </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L170" t="s">
+        <v>258</v>
+      </c>
+      <c r="M170">
+        <v>3.7895854E-2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>177</v>
       </c>
@@ -24689,8 +25718,14 @@
       <c r="K171">
         <v>5.0302154000000002E-2</v>
       </c>
-    </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L171" t="s">
+        <v>258</v>
+      </c>
+      <c r="M171">
+        <v>4.6335029E-2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>178</v>
       </c>
@@ -24727,8 +25762,14 @@
       <c r="K172">
         <v>3.0324325999999999E-2</v>
       </c>
-    </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L172" t="s">
+        <v>259</v>
+      </c>
+      <c r="M172">
+        <v>3.4005318999999999E-2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>179</v>
       </c>
@@ -24765,8 +25806,14 @@
       <c r="K173">
         <v>3.8286651999999997E-2</v>
       </c>
-    </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L173" t="s">
+        <v>259</v>
+      </c>
+      <c r="M173">
+        <v>4.2295168000000001E-2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>180</v>
       </c>
@@ -24803,8 +25850,14 @@
       <c r="K174">
         <v>769.98839477499996</v>
       </c>
-    </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L174" t="s">
+        <v>260</v>
+      </c>
+      <c r="M174">
+        <v>901.84394919500005</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>181</v>
       </c>
@@ -24841,8 +25894,14 @@
       <c r="K175">
         <v>901.86916701099994</v>
       </c>
-    </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L175" t="s">
+        <v>261</v>
+      </c>
+      <c r="M175">
+        <v>268.17617553500003</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>182</v>
       </c>
@@ -24879,8 +25938,14 @@
       <c r="K176">
         <v>901.76872275699998</v>
       </c>
-    </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L176" t="s">
+        <v>261</v>
+      </c>
+      <c r="M176">
+        <v>261.95835160299998</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>183</v>
       </c>
@@ -24917,8 +25982,14 @@
       <c r="K177">
         <v>741.17950797200001</v>
       </c>
-    </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L177" t="s">
+        <v>261</v>
+      </c>
+      <c r="M177">
+        <v>345.43369718500003</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>184</v>
       </c>
@@ -24955,8 +26026,14 @@
       <c r="K178">
         <v>901.76020160200005</v>
       </c>
-    </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L178" t="s">
+        <v>261</v>
+      </c>
+      <c r="M178">
+        <v>209.84469724499999</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>185</v>
       </c>
@@ -24993,8 +26070,14 @@
       <c r="K179">
         <v>901.756485365</v>
       </c>
-    </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L179" t="s">
+        <v>261</v>
+      </c>
+      <c r="M179">
+        <v>361.64644872700001</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>186</v>
       </c>
@@ -25031,8 +26114,14 @@
       <c r="K180">
         <v>901.77149635399996</v>
       </c>
-    </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L180" t="s">
+        <v>261</v>
+      </c>
+      <c r="M180">
+        <v>423.08887849600001</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>187</v>
       </c>
@@ -25069,8 +26158,14 @@
       <c r="K181">
         <v>901.85071537800002</v>
       </c>
-    </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L181" t="s">
+        <v>260</v>
+      </c>
+      <c r="M181">
+        <v>901.82741969400001</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>188</v>
       </c>
@@ -25107,8 +26202,14 @@
       <c r="K182">
         <v>901.86908341799995</v>
       </c>
-    </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L182" t="s">
+        <v>261</v>
+      </c>
+      <c r="M182">
+        <v>331.86981630399998</v>
+      </c>
+    </row>
+    <row r="183" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>189</v>
       </c>
@@ -25145,8 +26246,14 @@
       <c r="K183">
         <v>55.103477781000002</v>
       </c>
-    </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L183" t="s">
+        <v>261</v>
+      </c>
+      <c r="M183">
+        <v>209.080923345</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>190</v>
       </c>
@@ -25183,8 +26290,14 @@
       <c r="K184">
         <v>257.440989333</v>
       </c>
-    </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L184" t="s">
+        <v>260</v>
+      </c>
+      <c r="M184">
+        <v>901.821976683</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>191</v>
       </c>
@@ -25221,8 +26334,14 @@
       <c r="K185">
         <v>901.76961090600003</v>
       </c>
-    </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L185" t="s">
+        <v>260</v>
+      </c>
+      <c r="M185">
+        <v>901.90221757999996</v>
+      </c>
+    </row>
+    <row r="186" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>192</v>
       </c>
@@ -25259,8 +26378,14 @@
       <c r="K186">
         <v>901.64223485399998</v>
       </c>
-    </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L186" t="s">
+        <v>260</v>
+      </c>
+      <c r="M186">
+        <v>901.65419067799996</v>
+      </c>
+    </row>
+    <row r="187" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>193</v>
       </c>
@@ -25297,8 +26422,14 @@
       <c r="K187">
         <v>901.78804368099998</v>
       </c>
-    </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L187" t="s">
+        <v>260</v>
+      </c>
+      <c r="M187">
+        <v>901.78661057600004</v>
+      </c>
+    </row>
+    <row r="188" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>194</v>
       </c>
@@ -25335,8 +26466,14 @@
       <c r="K188">
         <v>901.69962024100005</v>
       </c>
-    </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L188" t="s">
+        <v>260</v>
+      </c>
+      <c r="M188">
+        <v>901.68789050199996</v>
+      </c>
+    </row>
+    <row r="189" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>195</v>
       </c>
@@ -25373,8 +26510,14 @@
       <c r="K189">
         <v>467.523635555</v>
       </c>
-    </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L189" t="s">
+        <v>261</v>
+      </c>
+      <c r="M189">
+        <v>462.71311323999998</v>
+      </c>
+    </row>
+    <row r="190" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>196</v>
       </c>
@@ -25411,8 +26554,14 @@
       <c r="K190">
         <v>901.71441550099996</v>
       </c>
-    </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L190" t="s">
+        <v>261</v>
+      </c>
+      <c r="M190">
+        <v>374.06800933400001</v>
+      </c>
+    </row>
+    <row r="191" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>197</v>
       </c>
@@ -25449,8 +26598,14 @@
       <c r="K191">
         <v>901.73527085900002</v>
       </c>
-    </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L191" t="s">
+        <v>261</v>
+      </c>
+      <c r="M191">
+        <v>376.31528081800002</v>
+      </c>
+    </row>
+    <row r="192" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>198</v>
       </c>
@@ -25487,8 +26642,14 @@
       <c r="K192">
         <v>901.747269684</v>
       </c>
-    </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L192" t="s">
+        <v>261</v>
+      </c>
+      <c r="M192">
+        <v>377.71510604000002</v>
+      </c>
+    </row>
+    <row r="193" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>199</v>
       </c>
@@ -25525,8 +26686,14 @@
       <c r="K193">
         <v>901.715041402</v>
       </c>
-    </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L193" t="s">
+        <v>261</v>
+      </c>
+      <c r="M193">
+        <v>377.81247649099998</v>
+      </c>
+    </row>
+    <row r="194" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>200</v>
       </c>
@@ -25563,8 +26730,14 @@
       <c r="K194">
         <v>901.77949609799998</v>
       </c>
-    </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L194" t="s">
+        <v>261</v>
+      </c>
+      <c r="M194">
+        <v>375.631682012</v>
+      </c>
+    </row>
+    <row r="195" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>201</v>
       </c>
@@ -25601,8 +26774,14 @@
       <c r="K195">
         <v>901.73674081399997</v>
       </c>
-    </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L195" t="s">
+        <v>261</v>
+      </c>
+      <c r="M195">
+        <v>374.189628981</v>
+      </c>
+    </row>
+    <row r="196" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>202</v>
       </c>
@@ -25639,8 +26818,14 @@
       <c r="K196">
         <v>901.75392615099997</v>
       </c>
-    </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L196" t="s">
+        <v>261</v>
+      </c>
+      <c r="M196">
+        <v>375.76876824499999</v>
+      </c>
+    </row>
+    <row r="197" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>203</v>
       </c>
@@ -25677,8 +26862,14 @@
       <c r="K197">
         <v>901.82650055199997</v>
       </c>
-    </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L197" t="s">
+        <v>261</v>
+      </c>
+      <c r="M197">
+        <v>377.18767766799999</v>
+      </c>
+    </row>
+    <row r="198" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>204</v>
       </c>
@@ -25715,8 +26906,14 @@
       <c r="K198">
         <v>901.63361996100002</v>
       </c>
-    </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L198" t="s">
+        <v>261</v>
+      </c>
+      <c r="M198">
+        <v>377.79432568999999</v>
+      </c>
+    </row>
+    <row r="199" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>205</v>
       </c>
@@ -25753,8 +26950,14 @@
       <c r="K199">
         <v>901.70436382299999</v>
       </c>
-    </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L199" t="s">
+        <v>261</v>
+      </c>
+      <c r="M199">
+        <v>378.33288976599999</v>
+      </c>
+    </row>
+    <row r="200" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>206</v>
       </c>
@@ -25791,8 +26994,14 @@
       <c r="K200">
         <v>901.74006081599998</v>
       </c>
-    </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L200" t="s">
+        <v>261</v>
+      </c>
+      <c r="M200">
+        <v>377.58575077299997</v>
+      </c>
+    </row>
+    <row r="201" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>207</v>
       </c>
@@ -25829,8 +27038,14 @@
       <c r="K201">
         <v>901.73175637199995</v>
       </c>
-    </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L201" t="s">
+        <v>261</v>
+      </c>
+      <c r="M201">
+        <v>374.63396084599998</v>
+      </c>
+    </row>
+    <row r="202" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>208</v>
       </c>
@@ -25867,8 +27082,14 @@
       <c r="K202">
         <v>901.83327375800002</v>
       </c>
-    </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L202" t="s">
+        <v>261</v>
+      </c>
+      <c r="M202">
+        <v>371.74990883800001</v>
+      </c>
+    </row>
+    <row r="203" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>209</v>
       </c>
@@ -25905,8 +27126,14 @@
       <c r="K203">
         <v>901.73711681700001</v>
       </c>
-    </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L203" t="s">
+        <v>261</v>
+      </c>
+      <c r="M203">
+        <v>375.531094338</v>
+      </c>
+    </row>
+    <row r="204" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>210</v>
       </c>
@@ -25943,8 +27170,14 @@
       <c r="K204">
         <v>901.66542882800002</v>
       </c>
-    </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L204" t="s">
+        <v>261</v>
+      </c>
+      <c r="M204">
+        <v>379.12666924899997</v>
+      </c>
+    </row>
+    <row r="205" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>211</v>
       </c>
@@ -25981,8 +27214,14 @@
       <c r="K205">
         <v>901.75164081900004</v>
       </c>
-    </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L205" t="s">
+        <v>260</v>
+      </c>
+      <c r="M205">
+        <v>901.92117202400004</v>
+      </c>
+    </row>
+    <row r="206" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>212</v>
       </c>
@@ -26019,8 +27258,14 @@
       <c r="K206">
         <v>901.76771768599997</v>
       </c>
-    </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L206" t="s">
+        <v>260</v>
+      </c>
+      <c r="M206">
+        <v>901.91152725899997</v>
+      </c>
+    </row>
+    <row r="207" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>213</v>
       </c>
@@ -26057,8 +27302,14 @@
       <c r="K207">
         <v>901.79881405799995</v>
       </c>
-    </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L207" t="s">
+        <v>260</v>
+      </c>
+      <c r="M207">
+        <v>901.93081161999999</v>
+      </c>
+    </row>
+    <row r="208" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>214</v>
       </c>
@@ -26095,8 +27346,14 @@
       <c r="K208">
         <v>901.781347396</v>
       </c>
-    </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L208" t="s">
+        <v>260</v>
+      </c>
+      <c r="M208">
+        <v>901.94422756799997</v>
+      </c>
+    </row>
+    <row r="209" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>215</v>
       </c>
@@ -26133,8 +27390,14 @@
       <c r="K209">
         <v>901.77370051399998</v>
       </c>
-    </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L209" t="s">
+        <v>260</v>
+      </c>
+      <c r="M209">
+        <v>901.97942791100002</v>
+      </c>
+    </row>
+    <row r="210" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>216</v>
       </c>
@@ -26171,8 +27434,14 @@
       <c r="K210">
         <v>901.68688885799997</v>
       </c>
-    </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L210" t="s">
+        <v>260</v>
+      </c>
+      <c r="M210">
+        <v>901.86674174899997</v>
+      </c>
+    </row>
+    <row r="211" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>217</v>
       </c>
@@ -26209,8 +27478,14 @@
       <c r="K211">
         <v>901.76737816100001</v>
       </c>
-    </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L211" t="s">
+        <v>260</v>
+      </c>
+      <c r="M211">
+        <v>901.91676658599999</v>
+      </c>
+    </row>
+    <row r="212" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>218</v>
       </c>
@@ -26247,8 +27522,14 @@
       <c r="K212">
         <v>901.79982269000004</v>
       </c>
-    </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L212" t="s">
+        <v>260</v>
+      </c>
+      <c r="M212">
+        <v>901.90377795400002</v>
+      </c>
+    </row>
+    <row r="213" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>219</v>
       </c>
@@ -26285,8 +27566,14 @@
       <c r="K213">
         <v>901.79130194000004</v>
       </c>
-    </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L213" t="s">
+        <v>260</v>
+      </c>
+      <c r="M213">
+        <v>901.922943465</v>
+      </c>
+    </row>
+    <row r="214" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>220</v>
       </c>
@@ -26323,8 +27610,14 @@
       <c r="K214">
         <v>901.76748331099998</v>
       </c>
-    </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L214" t="s">
+        <v>260</v>
+      </c>
+      <c r="M214">
+        <v>901.92663570499997</v>
+      </c>
+    </row>
+    <row r="215" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>221</v>
       </c>
@@ -26361,8 +27654,14 @@
       <c r="K215">
         <v>901.76484672499998</v>
       </c>
-    </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L215" t="s">
+        <v>260</v>
+      </c>
+      <c r="M215">
+        <v>901.93464306500005</v>
+      </c>
+    </row>
+    <row r="216" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>222</v>
       </c>
@@ -26399,8 +27698,14 @@
       <c r="K216">
         <v>901.68976871300003</v>
       </c>
-    </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L216" t="s">
+        <v>260</v>
+      </c>
+      <c r="M216">
+        <v>901.83585109000001</v>
+      </c>
+    </row>
+    <row r="217" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>223</v>
       </c>
@@ -26437,8 +27742,14 @@
       <c r="K217">
         <v>901.77858494899999</v>
       </c>
-    </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L217" t="s">
+        <v>260</v>
+      </c>
+      <c r="M217">
+        <v>901.90973408499997</v>
+      </c>
+    </row>
+    <row r="218" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>224</v>
       </c>
@@ -26475,8 +27786,14 @@
       <c r="K218">
         <v>901.79958156400005</v>
       </c>
-    </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L218" t="s">
+        <v>260</v>
+      </c>
+      <c r="M218">
+        <v>901.91082040000003</v>
+      </c>
+    </row>
+    <row r="219" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>225</v>
       </c>
@@ -26513,8 +27830,14 @@
       <c r="K219">
         <v>901.77187699700005</v>
       </c>
-    </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L219" t="s">
+        <v>260</v>
+      </c>
+      <c r="M219">
+        <v>901.90571349100003</v>
+      </c>
+    </row>
+    <row r="220" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>226</v>
       </c>
@@ -26551,8 +27874,14 @@
       <c r="K220">
         <v>901.80315471599999</v>
       </c>
-    </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L220" t="s">
+        <v>260</v>
+      </c>
+      <c r="M220">
+        <v>901.92103414999997</v>
+      </c>
+    </row>
+    <row r="221" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>227</v>
       </c>
@@ -26589,8 +27918,14 @@
       <c r="K221">
         <v>901.84143733600001</v>
       </c>
-    </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L221" t="s">
+        <v>260</v>
+      </c>
+      <c r="M221">
+        <v>901.93062413999996</v>
+      </c>
+    </row>
+    <row r="222" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>228</v>
       </c>
@@ -26627,8 +27962,14 @@
       <c r="K222">
         <v>901.80178486099999</v>
       </c>
-    </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L222" t="s">
+        <v>260</v>
+      </c>
+      <c r="M222">
+        <v>901.85482829800003</v>
+      </c>
+    </row>
+    <row r="223" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>229</v>
       </c>
@@ -26665,8 +28006,14 @@
       <c r="K223">
         <v>901.77595280000003</v>
       </c>
-    </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L223" t="s">
+        <v>260</v>
+      </c>
+      <c r="M223">
+        <v>901.90781900599995</v>
+      </c>
+    </row>
+    <row r="224" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>230</v>
       </c>
@@ -26703,8 +28050,14 @@
       <c r="K224">
         <v>901.77196169800004</v>
       </c>
-    </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L224" t="s">
+        <v>260</v>
+      </c>
+      <c r="M224">
+        <v>901.92949698300004</v>
+      </c>
+    </row>
+    <row r="225" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>231</v>
       </c>
@@ -26741,8 +28094,14 @@
       <c r="K225">
         <v>371.33832713800001</v>
       </c>
-    </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L225" t="s">
+        <v>261</v>
+      </c>
+      <c r="M225">
+        <v>289.82711357099998</v>
+      </c>
+    </row>
+    <row r="226" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>232</v>
       </c>
@@ -26779,8 +28138,14 @@
       <c r="K226">
         <v>454.83112910599999</v>
       </c>
-    </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L226" t="s">
+        <v>261</v>
+      </c>
+      <c r="M226">
+        <v>261.64033683299999</v>
+      </c>
+    </row>
+    <row r="227" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>233</v>
       </c>
@@ -26817,8 +28182,14 @@
       <c r="K227">
         <v>371.56725847799999</v>
       </c>
-    </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L227" t="s">
+        <v>261</v>
+      </c>
+      <c r="M227">
+        <v>288.73173312500001</v>
+      </c>
+    </row>
+    <row r="228" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>234</v>
       </c>
@@ -26855,8 +28226,14 @@
       <c r="K228">
         <v>730.10208583799999</v>
       </c>
-    </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L228" t="s">
+        <v>261</v>
+      </c>
+      <c r="M228">
+        <v>290.01823381899999</v>
+      </c>
+    </row>
+    <row r="229" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>235</v>
       </c>
@@ -26893,8 +28270,14 @@
       <c r="K229">
         <v>329.42737186599999</v>
       </c>
-    </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L229" t="s">
+        <v>261</v>
+      </c>
+      <c r="M229">
+        <v>285.29137780999997</v>
+      </c>
+    </row>
+    <row r="230" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>236</v>
       </c>
@@ -26931,8 +28314,14 @@
       <c r="K230">
         <v>305.02501225200001</v>
       </c>
-    </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L230" t="s">
+        <v>261</v>
+      </c>
+      <c r="M230">
+        <v>319.41944276800001</v>
+      </c>
+    </row>
+    <row r="231" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>237</v>
       </c>
@@ -26969,8 +28358,14 @@
       <c r="K231">
         <v>162.30105505099999</v>
       </c>
-    </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L231" t="s">
+        <v>261</v>
+      </c>
+      <c r="M231">
+        <v>288.70854226099999</v>
+      </c>
+    </row>
+    <row r="232" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>238</v>
       </c>
@@ -27007,8 +28402,14 @@
       <c r="K232">
         <v>138.43285567300001</v>
       </c>
-    </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L232" t="s">
+        <v>261</v>
+      </c>
+      <c r="M232">
+        <v>286.97308317699998</v>
+      </c>
+    </row>
+    <row r="233" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>239</v>
       </c>
@@ -27045,8 +28446,14 @@
       <c r="K233">
         <v>162.05643867000001</v>
       </c>
-    </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L233" t="s">
+        <v>261</v>
+      </c>
+      <c r="M233">
+        <v>289.080580467</v>
+      </c>
+    </row>
+    <row r="234" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>240</v>
       </c>
@@ -27083,8 +28490,14 @@
       <c r="K234">
         <v>184.71383831700001</v>
       </c>
-    </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L234" t="s">
+        <v>261</v>
+      </c>
+      <c r="M234">
+        <v>289.05284258699999</v>
+      </c>
+    </row>
+    <row r="235" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>241</v>
       </c>
@@ -27121,8 +28534,14 @@
       <c r="K235">
         <v>485.96650032500003</v>
       </c>
-    </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L235" t="s">
+        <v>261</v>
+      </c>
+      <c r="M235">
+        <v>287.98360920900001</v>
+      </c>
+    </row>
+    <row r="236" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>242</v>
       </c>
@@ -27159,8 +28578,14 @@
       <c r="K236">
         <v>506.60728759199998</v>
       </c>
-    </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L236" t="s">
+        <v>261</v>
+      </c>
+      <c r="M236">
+        <v>289.84519299999999</v>
+      </c>
+    </row>
+    <row r="237" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>243</v>
       </c>
@@ -27197,8 +28622,14 @@
       <c r="K237">
         <v>174.10308697799999</v>
       </c>
-    </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L237" t="s">
+        <v>261</v>
+      </c>
+      <c r="M237">
+        <v>288.87610143400002</v>
+      </c>
+    </row>
+    <row r="238" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>244</v>
       </c>
@@ -27235,8 +28666,14 @@
       <c r="K238">
         <v>312.89883269799998</v>
       </c>
-    </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L238" t="s">
+        <v>261</v>
+      </c>
+      <c r="M238">
+        <v>290.936869452</v>
+      </c>
+    </row>
+    <row r="239" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>245</v>
       </c>
@@ -27273,8 +28710,14 @@
       <c r="K239">
         <v>19.156269924</v>
       </c>
-    </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L239" t="s">
+        <v>261</v>
+      </c>
+      <c r="M239">
+        <v>428.650032603</v>
+      </c>
+    </row>
+    <row r="240" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>246</v>
       </c>
@@ -27311,8 +28754,14 @@
       <c r="K240">
         <v>60.335114814999997</v>
       </c>
-    </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L240" t="s">
+        <v>261</v>
+      </c>
+      <c r="M240">
+        <v>426.40971004800002</v>
+      </c>
+    </row>
+    <row r="241" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>247</v>
       </c>
@@ -27349,8 +28798,14 @@
       <c r="K241">
         <v>12.271280215000001</v>
       </c>
-    </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L241" t="s">
+        <v>261</v>
+      </c>
+      <c r="M241">
+        <v>435.57989258100002</v>
+      </c>
+    </row>
+    <row r="242" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>248</v>
       </c>
@@ -27387,8 +28842,14 @@
       <c r="K242">
         <v>57.808759506999998</v>
       </c>
-    </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L242" t="s">
+        <v>261</v>
+      </c>
+      <c r="M242">
+        <v>427.64882749999998</v>
+      </c>
+    </row>
+    <row r="243" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>249</v>
       </c>
@@ -27425,8 +28886,14 @@
       <c r="K243">
         <v>44.571291410999997</v>
       </c>
-    </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L243" t="s">
+        <v>261</v>
+      </c>
+      <c r="M243">
+        <v>430.58283936700002</v>
+      </c>
+    </row>
+    <row r="244" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>250</v>
       </c>
@@ -27463,8 +28930,14 @@
       <c r="K244">
         <v>26.449746823000002</v>
       </c>
-    </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L244" t="s">
+        <v>261</v>
+      </c>
+      <c r="M244">
+        <v>433.05533016999999</v>
+      </c>
+    </row>
+    <row r="245" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>251</v>
       </c>
@@ -27501,8 +28974,14 @@
       <c r="K245">
         <v>437.50447653800001</v>
       </c>
-    </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L245" t="s">
+        <v>261</v>
+      </c>
+      <c r="M245">
+        <v>394.80382305000001</v>
+      </c>
+    </row>
+    <row r="246" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>252</v>
       </c>
@@ -27539,8 +29018,14 @@
       <c r="K246">
         <v>178.65229049000001</v>
       </c>
-    </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L246" t="s">
+        <v>261</v>
+      </c>
+      <c r="M246">
+        <v>412.05375456199999</v>
+      </c>
+    </row>
+    <row r="247" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>253</v>
       </c>
@@ -27577,8 +29062,14 @@
       <c r="K247">
         <v>391.47916637399999</v>
       </c>
-    </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L247" t="s">
+        <v>261</v>
+      </c>
+      <c r="M247">
+        <v>413.80258595700002</v>
+      </c>
+    </row>
+    <row r="248" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>254</v>
       </c>
@@ -27615,8 +29106,14 @@
       <c r="K248">
         <v>101.837434782</v>
       </c>
-    </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L248" t="s">
+        <v>259</v>
+      </c>
+      <c r="M248">
+        <v>80.725753695999998</v>
+      </c>
+    </row>
+    <row r="249" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>255</v>
       </c>
@@ -27653,8 +29150,14 @@
       <c r="K249">
         <v>80.292722706000006</v>
       </c>
-    </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L249" t="s">
+        <v>259</v>
+      </c>
+      <c r="M249">
+        <v>61.576339271999998</v>
+      </c>
+    </row>
+    <row r="251" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>275</v>
       </c>
@@ -27678,8 +29181,36 @@
         <f>COUNTIF(J4:J249,"sat") + COUNTIF(J4:J249,"unsat")</f>
         <v>94</v>
       </c>
+      <c r="L251">
+        <f>COUNTIF(L4:L249,"sat") + COUNTIF(L4:L249,"unsat")</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="252" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A252" t="s">
+        <v>277</v>
+      </c>
+      <c r="B252">
+        <v>1</v>
+      </c>
+      <c r="D252">
+        <v>0</v>
+      </c>
+      <c r="F252">
+        <v>22</v>
+      </c>
+      <c r="H252">
+        <v>9</v>
+      </c>
+      <c r="J252">
+        <v>13</v>
+      </c>
+      <c r="L252">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M252" xr:uid="{35486B71-12BE-2349-B57A-22BC9F8DFAFE}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -27688,8 +29219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{130FAACC-10E2-5C4D-978B-741FB3F1F2DB}">
   <dimension ref="A1:Q251"/>
   <sheetViews>
-    <sheetView topLeftCell="F86" workbookViewId="0">
-      <selection activeCell="A251" sqref="A251"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -40923,6 +42454,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Q251" xr:uid="{ADAA83BD-86BC-1C44-910D-ABC33C82A2EE}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removed old stuff, bumped version of DQBDD to 1.0
</commit_message>
<xml_diff>
--- a/results/combinedresults/dqbf19.xlsx
+++ b/results/combinedresults/dqbf19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jurajsic/OneDrive/skola/magisterFI/diplomka/DQBFbenchmarks/results/combinedresults/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8D53FE-FA69-3A40-B78B-216275AB740F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACEA778-CCC5-574B-B309-16071AFFEFEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="940" windowWidth="27640" windowHeight="15360" activeTab="1" xr2:uid="{5DD0E6D6-7882-E44F-A577-7B002FAE22A9}"/>
   </bookViews>
@@ -19,9 +19,9 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">dqbdd!$A$1:$Q$251</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">realtime!$A$1:$M$252</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">realtime!$A$1:$O$249</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4587" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4839" uniqueCount="280">
   <si>
     <t>tool</t>
   </si>
@@ -874,6 +874,12 @@
   <si>
     <t>uniquely solved (this is wrong, needs to remove DQBDD tree)</t>
   </si>
+  <si>
+    <t>DQBDDdynreorder 0.5</t>
+  </si>
+  <si>
+    <t>tree-simpleelimination-atbeginning.dqbf19</t>
+  </si>
 </sst>
 </file>
 
@@ -897,12 +903,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -917,10 +929,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -18192,10 +18205,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E88B51B-86D8-E547-9986-F518581AF70F}">
-  <dimension ref="A1:M252"/>
+  <dimension ref="A1:O252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="F253" sqref="F253"/>
+    <sheetView tabSelected="1" topLeftCell="A240" workbookViewId="0">
+      <selection activeCell="E257" sqref="E257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18210,7 +18223,7 @@
     <col min="13" max="13" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -18250,8 +18263,14 @@
       <c r="M1" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" t="s">
+        <v>278</v>
+      </c>
+      <c r="O1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -18291,8 +18310,14 @@
       <c r="M2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" t="s">
+        <v>279</v>
+      </c>
+      <c r="O2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -18332,8 +18357,14 @@
       <c r="M3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -18376,8 +18407,14 @@
       <c r="M4">
         <v>901.68670359700002</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4" t="s">
+        <v>260</v>
+      </c>
+      <c r="O4">
+        <v>901.59526907199995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -18420,8 +18457,14 @@
       <c r="M5">
         <v>901.90349689799996</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5" t="s">
+        <v>260</v>
+      </c>
+      <c r="O5">
+        <v>901.68137087800005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -18464,8 +18507,14 @@
       <c r="M6">
         <v>901.79542871900003</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N6" t="s">
+        <v>260</v>
+      </c>
+      <c r="O6">
+        <v>901.68901847200004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -18508,8 +18557,14 @@
       <c r="M7">
         <v>901.89486329900001</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N7" t="s">
+        <v>260</v>
+      </c>
+      <c r="O7">
+        <v>901.68149446799998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -18552,8 +18607,14 @@
       <c r="M8">
         <v>901.81605079200006</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N8" t="s">
+        <v>260</v>
+      </c>
+      <c r="O8">
+        <v>901.68913957200004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -18596,8 +18657,14 @@
       <c r="M9">
         <v>421.68146624600001</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N9" t="s">
+        <v>260</v>
+      </c>
+      <c r="O9">
+        <v>901.68257421999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -18640,8 +18707,14 @@
       <c r="M10">
         <v>0.45031598499999997</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N10" t="s">
+        <v>258</v>
+      </c>
+      <c r="O10">
+        <v>2.070356072</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -18684,8 +18757,14 @@
       <c r="M11">
         <v>0.47832879</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N11" t="s">
+        <v>258</v>
+      </c>
+      <c r="O11">
+        <v>0.41736634299999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -18728,8 +18807,14 @@
       <c r="M12">
         <v>23.979405363000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N12" t="s">
+        <v>261</v>
+      </c>
+      <c r="O12">
+        <v>30.614210404000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -18772,8 +18857,14 @@
       <c r="M13">
         <v>901.74665096599995</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N13" t="s">
+        <v>261</v>
+      </c>
+      <c r="O13">
+        <v>28.97162921</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -18816,8 +18907,14 @@
       <c r="M14">
         <v>9.5362682000000004E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N14" t="s">
+        <v>258</v>
+      </c>
+      <c r="O14">
+        <v>0.154041598</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -18860,8 +18957,14 @@
       <c r="M15">
         <v>0.17877522900000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N15" t="s">
+        <v>258</v>
+      </c>
+      <c r="O15">
+        <v>0.20656339900000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -18904,8 +19007,14 @@
       <c r="M16">
         <v>92.409753330000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N16" t="s">
+        <v>260</v>
+      </c>
+      <c r="O16">
+        <v>901.68263391599999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -18948,8 +19057,14 @@
       <c r="M17">
         <v>93.809883024000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N17" t="s">
+        <v>260</v>
+      </c>
+      <c r="O17">
+        <v>901.69493192599998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -18992,8 +19107,14 @@
       <c r="M18">
         <v>91.721492924000003</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N18" t="s">
+        <v>260</v>
+      </c>
+      <c r="O18">
+        <v>901.68258542000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -19036,8 +19157,14 @@
       <c r="M19">
         <v>91.176365832000002</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N19" t="s">
+        <v>260</v>
+      </c>
+      <c r="O19">
+        <v>901.67707102700001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -19080,8 +19207,14 @@
       <c r="M20">
         <v>90.853693308000004</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N20" t="s">
+        <v>260</v>
+      </c>
+      <c r="O20">
+        <v>901.67795031900005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -19124,8 +19257,14 @@
       <c r="M21">
         <v>91.237849724</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N21" t="s">
+        <v>260</v>
+      </c>
+      <c r="O21">
+        <v>901.57475779200001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -19168,8 +19307,14 @@
       <c r="M22">
         <v>91.784116010000005</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N22" t="s">
+        <v>260</v>
+      </c>
+      <c r="O22">
+        <v>901.69468668000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -19212,8 +19357,14 @@
       <c r="M23">
         <v>90.638299919999994</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N23" t="s">
+        <v>260</v>
+      </c>
+      <c r="O23">
+        <v>901.68305591900003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -19256,8 +19407,14 @@
       <c r="M24">
         <v>91.654322741000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N24" t="s">
+        <v>260</v>
+      </c>
+      <c r="O24">
+        <v>901.67887450299997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -19300,8 +19457,14 @@
       <c r="M25">
         <v>91.592912287999994</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N25" t="s">
+        <v>260</v>
+      </c>
+      <c r="O25">
+        <v>901.69334602799995</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -19344,8 +19507,14 @@
       <c r="M26">
         <v>90.888190644000005</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N26" t="s">
+        <v>260</v>
+      </c>
+      <c r="O26">
+        <v>901.67823582000005</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -19388,8 +19557,14 @@
       <c r="M27">
         <v>91.985865378</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N27" t="s">
+        <v>260</v>
+      </c>
+      <c r="O27">
+        <v>901.58139770499997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -19432,8 +19607,14 @@
       <c r="M28">
         <v>91.534013588999997</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N28" t="s">
+        <v>260</v>
+      </c>
+      <c r="O28">
+        <v>901.69094606399995</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -19476,8 +19657,14 @@
       <c r="M29">
         <v>92.075464421000007</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N29" t="s">
+        <v>260</v>
+      </c>
+      <c r="O29">
+        <v>901.68422930999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -19520,8 +19707,14 @@
       <c r="M30">
         <v>92.121324090000002</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N30" t="s">
+        <v>260</v>
+      </c>
+      <c r="O30">
+        <v>901.85360275000005</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -19564,8 +19757,14 @@
       <c r="M31">
         <v>202.88463577600001</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N31" t="s">
+        <v>261</v>
+      </c>
+      <c r="O31">
+        <v>126.94009105000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -19608,8 +19807,14 @@
       <c r="M32">
         <v>165.697857863</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N32" t="s">
+        <v>260</v>
+      </c>
+      <c r="O32">
+        <v>901.68150620400002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -19652,8 +19857,14 @@
       <c r="M33">
         <v>167.18481085499999</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N33" t="s">
+        <v>260</v>
+      </c>
+      <c r="O33">
+        <v>901.58122215499998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -19696,8 +19907,14 @@
       <c r="M34">
         <v>103.07008250299999</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N34" t="s">
+        <v>260</v>
+      </c>
+      <c r="O34">
+        <v>901.734211093</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -19740,8 +19957,14 @@
       <c r="M35">
         <v>0.161592448</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N35" t="s">
+        <v>258</v>
+      </c>
+      <c r="O35">
+        <v>0.56962020199999996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -19784,8 +20007,14 @@
       <c r="M36">
         <v>82.790511073000005</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N36" t="s">
+        <v>260</v>
+      </c>
+      <c r="O36">
+        <v>901.67466418100003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -19828,8 +20057,14 @@
       <c r="M37">
         <v>82.025603649000004</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N37" t="s">
+        <v>260</v>
+      </c>
+      <c r="O37">
+        <v>901.67030162499998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -19872,8 +20107,14 @@
       <c r="M38">
         <v>2.1929276000000001E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N38" t="s">
+        <v>258</v>
+      </c>
+      <c r="O38">
+        <v>2.5603056999999999E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -19916,8 +20157,14 @@
       <c r="M39">
         <v>0.137990378</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N39" t="s">
+        <v>258</v>
+      </c>
+      <c r="O39">
+        <v>4.1543044000000001E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -19960,8 +20207,14 @@
       <c r="M40">
         <v>0.13767146299999999</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N40" t="s">
+        <v>258</v>
+      </c>
+      <c r="O40">
+        <v>4.1805202999999999E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -20004,8 +20257,14 @@
       <c r="M41">
         <v>901.56078541399995</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N41" t="s">
+        <v>258</v>
+      </c>
+      <c r="O41">
+        <v>5.7678350000000003E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -20048,8 +20307,14 @@
       <c r="M42">
         <v>0.67040133700000004</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N42" t="s">
+        <v>260</v>
+      </c>
+      <c r="O42">
+        <v>901.67670410699998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -20092,8 +20357,14 @@
       <c r="M43">
         <v>93.938432625000004</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N43" t="s">
+        <v>260</v>
+      </c>
+      <c r="O43">
+        <v>901.69029959800002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>50</v>
       </c>
@@ -20136,8 +20407,14 @@
       <c r="M44">
         <v>90.971360128000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N44" t="s">
+        <v>260</v>
+      </c>
+      <c r="O44">
+        <v>901.59100276300001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>51</v>
       </c>
@@ -20180,8 +20457,14 @@
       <c r="M45">
         <v>91.344669027999998</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N45" t="s">
+        <v>260</v>
+      </c>
+      <c r="O45">
+        <v>901.69021657999997</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -20224,8 +20507,14 @@
       <c r="M46">
         <v>91.160639545999999</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N46" t="s">
+        <v>260</v>
+      </c>
+      <c r="O46">
+        <v>901.68140578099997</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>53</v>
       </c>
@@ -20268,8 +20557,14 @@
       <c r="M47">
         <v>93.906236213</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N47" t="s">
+        <v>260</v>
+      </c>
+      <c r="O47">
+        <v>901.67968896599996</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>54</v>
       </c>
@@ -20312,8 +20607,14 @@
       <c r="M48">
         <v>91.475795821999995</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N48" t="s">
+        <v>260</v>
+      </c>
+      <c r="O48">
+        <v>901.68744299499997</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -20356,8 +20657,14 @@
       <c r="M49">
         <v>91.791674111000006</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N49" t="s">
+        <v>260</v>
+      </c>
+      <c r="O49">
+        <v>901.67303396600005</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -20400,8 +20707,14 @@
       <c r="M50">
         <v>93.879619138999999</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N50" t="s">
+        <v>260</v>
+      </c>
+      <c r="O50">
+        <v>901.58764492700004</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>57</v>
       </c>
@@ -20444,8 +20757,14 @@
       <c r="M51">
         <v>90.636046754999995</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N51" t="s">
+        <v>260</v>
+      </c>
+      <c r="O51">
+        <v>901.69431472099996</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -20488,8 +20807,14 @@
       <c r="M52">
         <v>94.194321392999996</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N52" t="s">
+        <v>260</v>
+      </c>
+      <c r="O52">
+        <v>901.68065193899997</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -20532,8 +20857,14 @@
       <c r="M53">
         <v>91.278266833999993</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N53" t="s">
+        <v>260</v>
+      </c>
+      <c r="O53">
+        <v>901.68171992999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>60</v>
       </c>
@@ -20576,8 +20907,14 @@
       <c r="M54">
         <v>91.701483087</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N54" t="s">
+        <v>260</v>
+      </c>
+      <c r="O54">
+        <v>901.68471515800002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>61</v>
       </c>
@@ -20620,8 +20957,14 @@
       <c r="M55">
         <v>90.979492633000007</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N55" t="s">
+        <v>260</v>
+      </c>
+      <c r="O55">
+        <v>901.676870689</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>62</v>
       </c>
@@ -20664,8 +21007,14 @@
       <c r="M56">
         <v>93.137301840999996</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N56" t="s">
+        <v>260</v>
+      </c>
+      <c r="O56">
+        <v>901.58144754199998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -20708,8 +21057,14 @@
       <c r="M57">
         <v>92.193087313999996</v>
       </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N57" t="s">
+        <v>260</v>
+      </c>
+      <c r="O57">
+        <v>901.69825049099995</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>64</v>
       </c>
@@ -20752,8 +21107,14 @@
       <c r="M58">
         <v>91.031792881000001</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N58" t="s">
+        <v>260</v>
+      </c>
+      <c r="O58">
+        <v>901.68189935999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>65</v>
       </c>
@@ -20796,8 +21157,14 @@
       <c r="M59">
         <v>91.584884463999998</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N59" t="s">
+        <v>260</v>
+      </c>
+      <c r="O59">
+        <v>901.88093544799995</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -20840,8 +21207,14 @@
       <c r="M60">
         <v>92.017093083999995</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N60" t="s">
+        <v>260</v>
+      </c>
+      <c r="O60">
+        <v>901.69431458199995</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>67</v>
       </c>
@@ -20884,8 +21257,14 @@
       <c r="M61">
         <v>92.826517652000007</v>
       </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N61" t="s">
+        <v>260</v>
+      </c>
+      <c r="O61">
+        <v>901.67743134</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>68</v>
       </c>
@@ -20928,8 +21307,14 @@
       <c r="M62">
         <v>92.103174640000006</v>
       </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N62" t="s">
+        <v>260</v>
+      </c>
+      <c r="O62">
+        <v>901.59156699000005</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>69</v>
       </c>
@@ -20972,8 +21357,14 @@
       <c r="M63">
         <v>113.311629457</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N63" t="s">
+        <v>260</v>
+      </c>
+      <c r="O63">
+        <v>901.67590612900005</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>70</v>
       </c>
@@ -21016,8 +21407,14 @@
       <c r="M64">
         <v>92.565266691999994</v>
       </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N64" t="s">
+        <v>260</v>
+      </c>
+      <c r="O64">
+        <v>901.67078162400003</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>71</v>
       </c>
@@ -21060,8 +21457,14 @@
       <c r="M65">
         <v>154.59128110200001</v>
       </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N65" t="s">
+        <v>260</v>
+      </c>
+      <c r="O65">
+        <v>901.80260568599999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>72</v>
       </c>
@@ -21104,8 +21507,14 @@
       <c r="M66">
         <v>95.985286135999999</v>
       </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N66" t="s">
+        <v>260</v>
+      </c>
+      <c r="O66">
+        <v>901.67254702699995</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>73</v>
       </c>
@@ -21148,8 +21557,14 @@
       <c r="M67">
         <v>95.700674887999995</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N67" t="s">
+        <v>260</v>
+      </c>
+      <c r="O67">
+        <v>901.66587745100003</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>74</v>
       </c>
@@ -21192,8 +21607,14 @@
       <c r="M68">
         <v>90.772248934000004</v>
       </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N68" t="s">
+        <v>260</v>
+      </c>
+      <c r="O68">
+        <v>901.580934028</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>75</v>
       </c>
@@ -21236,8 +21657,14 @@
       <c r="M69">
         <v>92.201844096000002</v>
       </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N69" t="s">
+        <v>260</v>
+      </c>
+      <c r="O69">
+        <v>901.68599808500005</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>76</v>
       </c>
@@ -21280,8 +21707,14 @@
       <c r="M70">
         <v>90.726496840999999</v>
       </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N70" t="s">
+        <v>260</v>
+      </c>
+      <c r="O70">
+        <v>901.67788838000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>77</v>
       </c>
@@ -21324,8 +21757,14 @@
       <c r="M71">
         <v>92.466103903999993</v>
       </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N71" t="s">
+        <v>260</v>
+      </c>
+      <c r="O71">
+        <v>901.68088149499999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>78</v>
       </c>
@@ -21368,8 +21807,14 @@
       <c r="M72">
         <v>91.160605329999996</v>
       </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N72" t="s">
+        <v>260</v>
+      </c>
+      <c r="O72">
+        <v>901.67130020000002</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>79</v>
       </c>
@@ -21412,8 +21857,14 @@
       <c r="M73">
         <v>90.902817323999997</v>
       </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N73" t="s">
+        <v>260</v>
+      </c>
+      <c r="O73">
+        <v>901.67104243100005</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>80</v>
       </c>
@@ -21456,8 +21907,14 @@
       <c r="M74">
         <v>92.525009983999993</v>
       </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N74" t="s">
+        <v>260</v>
+      </c>
+      <c r="O74">
+        <v>901.58439810000004</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>81</v>
       </c>
@@ -21500,8 +21957,14 @@
       <c r="M75">
         <v>91.462876562999995</v>
       </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N75" t="s">
+        <v>260</v>
+      </c>
+      <c r="O75">
+        <v>901.68229820700003</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>82</v>
       </c>
@@ -21544,8 +22007,14 @@
       <c r="M76">
         <v>92.025858726999999</v>
       </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N76" t="s">
+        <v>260</v>
+      </c>
+      <c r="O76">
+        <v>901.67932259999998</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>83</v>
       </c>
@@ -21588,8 +22057,14 @@
       <c r="M77">
         <v>91.247291001999997</v>
       </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N77" t="s">
+        <v>260</v>
+      </c>
+      <c r="O77">
+        <v>901.76139962599996</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>84</v>
       </c>
@@ -21632,8 +22107,14 @@
       <c r="M78">
         <v>91.026988492000001</v>
       </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N78" t="s">
+        <v>260</v>
+      </c>
+      <c r="O78">
+        <v>901.68059708299995</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>85</v>
       </c>
@@ -21676,8 +22157,14 @@
       <c r="M79">
         <v>93.426645770999997</v>
       </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N79" t="s">
+        <v>260</v>
+      </c>
+      <c r="O79">
+        <v>901.67370722600003</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>86</v>
       </c>
@@ -21720,8 +22207,14 @@
       <c r="M80">
         <v>92.640763108000002</v>
       </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N80" t="s">
+        <v>260</v>
+      </c>
+      <c r="O80">
+        <v>901.59967246500003</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>87</v>
       </c>
@@ -21764,8 +22257,14 @@
       <c r="M81">
         <v>317.95066357600001</v>
       </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N81" t="s">
+        <v>260</v>
+      </c>
+      <c r="O81">
+        <v>901.72358189399995</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>88</v>
       </c>
@@ -21808,8 +22307,14 @@
       <c r="M82">
         <v>102.672164391</v>
       </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N82" t="s">
+        <v>261</v>
+      </c>
+      <c r="O82">
+        <v>31.385897324999998</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>89</v>
       </c>
@@ -21852,8 +22357,14 @@
       <c r="M83">
         <v>96.000258054</v>
       </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N83" t="s">
+        <v>261</v>
+      </c>
+      <c r="O83">
+        <v>33.62158883</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>90</v>
       </c>
@@ -21896,8 +22407,14 @@
       <c r="M84">
         <v>3.3530022E-2</v>
       </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N84" t="s">
+        <v>258</v>
+      </c>
+      <c r="O84">
+        <v>4.2561348999999998E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>91</v>
       </c>
@@ -21940,8 +22457,14 @@
       <c r="M85">
         <v>14.500450731999999</v>
       </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N85" t="s">
+        <v>260</v>
+      </c>
+      <c r="O85">
+        <v>901.67571983799996</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>92</v>
       </c>
@@ -21984,8 +22507,14 @@
       <c r="M86">
         <v>184.11971844000001</v>
       </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N86" t="s">
+        <v>261</v>
+      </c>
+      <c r="O86">
+        <v>30.60407962</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>93</v>
       </c>
@@ -22028,8 +22557,14 @@
       <c r="M87">
         <v>2.5819676999999999E-2</v>
       </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N87" t="s">
+        <v>258</v>
+      </c>
+      <c r="O87">
+        <v>3.0734510999999999E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>94</v>
       </c>
@@ -22072,8 +22607,14 @@
       <c r="M88">
         <v>81.877951225999993</v>
       </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N88" t="s">
+        <v>261</v>
+      </c>
+      <c r="O88">
+        <v>32.181821264</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>95</v>
       </c>
@@ -22116,8 +22657,14 @@
       <c r="M89">
         <v>144.163868511</v>
       </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N89" t="s">
+        <v>261</v>
+      </c>
+      <c r="O89">
+        <v>31.209115111999999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>96</v>
       </c>
@@ -22160,8 +22707,14 @@
       <c r="M90">
         <v>0.598268727</v>
       </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N90" t="s">
+        <v>258</v>
+      </c>
+      <c r="O90">
+        <v>0.14254178300000001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>97</v>
       </c>
@@ -22204,8 +22757,14 @@
       <c r="M91">
         <v>0.58231676499999996</v>
       </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N91" t="s">
+        <v>258</v>
+      </c>
+      <c r="O91">
+        <v>0.254744533</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>98</v>
       </c>
@@ -22248,8 +22807,14 @@
       <c r="M92">
         <v>52.752273367000001</v>
       </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N92" t="s">
+        <v>258</v>
+      </c>
+      <c r="O92">
+        <v>18.504042072000001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>99</v>
       </c>
@@ -22292,8 +22857,14 @@
       <c r="M93">
         <v>721.47601106000002</v>
       </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N93" t="s">
+        <v>260</v>
+      </c>
+      <c r="O93">
+        <v>901.68831827999998</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>100</v>
       </c>
@@ -22336,8 +22907,14 @@
       <c r="M94">
         <v>895.03549405399997</v>
       </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N94" t="s">
+        <v>260</v>
+      </c>
+      <c r="O94">
+        <v>901.68317130399998</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>101</v>
       </c>
@@ -22380,8 +22957,14 @@
       <c r="M95">
         <v>901.86282717799997</v>
       </c>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N95" t="s">
+        <v>260</v>
+      </c>
+      <c r="O95">
+        <v>901.68648981900003</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>102</v>
       </c>
@@ -22424,8 +23007,14 @@
       <c r="M96">
         <v>901.85668597999995</v>
       </c>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N96" t="s">
+        <v>260</v>
+      </c>
+      <c r="O96">
+        <v>901.60406895999995</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>103</v>
       </c>
@@ -22468,8 +23057,14 @@
       <c r="M97">
         <v>901.70146854999996</v>
       </c>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N97" t="s">
+        <v>261</v>
+      </c>
+      <c r="O97">
+        <v>101.657824597</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>104</v>
       </c>
@@ -22512,8 +23107,14 @@
       <c r="M98">
         <v>901.75112388699995</v>
       </c>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N98" t="s">
+        <v>258</v>
+      </c>
+      <c r="O98">
+        <v>50.117705860000001</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>105</v>
       </c>
@@ -22556,8 +23157,14 @@
       <c r="M99">
         <v>285.64037744199999</v>
       </c>
-    </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N99" t="s">
+        <v>259</v>
+      </c>
+      <c r="O99">
+        <v>13.208341982</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>106</v>
       </c>
@@ -22600,8 +23207,14 @@
       <c r="M100">
         <v>0.101749882</v>
       </c>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N100" t="s">
+        <v>258</v>
+      </c>
+      <c r="O100">
+        <v>18.855791749000002</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>107</v>
       </c>
@@ -22644,8 +23257,14 @@
       <c r="M101">
         <v>289.01687954900001</v>
       </c>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N101" t="s">
+        <v>259</v>
+      </c>
+      <c r="O101">
+        <v>19.18431996</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>108</v>
       </c>
@@ -22688,8 +23307,14 @@
       <c r="M102">
         <v>0.12996542699999999</v>
       </c>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N102" t="s">
+        <v>259</v>
+      </c>
+      <c r="O102">
+        <v>0.129693421</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>109</v>
       </c>
@@ -22732,8 +23357,14 @@
       <c r="M103">
         <v>901.73639270800004</v>
       </c>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N103" t="s">
+        <v>260</v>
+      </c>
+      <c r="O103">
+        <v>901.7419208</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>110</v>
       </c>
@@ -22776,8 +23407,14 @@
       <c r="M104">
         <v>901.80911093600002</v>
       </c>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N104" t="s">
+        <v>260</v>
+      </c>
+      <c r="O104">
+        <v>901.82300339200003</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>111</v>
       </c>
@@ -22820,8 +23457,14 @@
       <c r="M105">
         <v>758.21690201199999</v>
       </c>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N105" t="s">
+        <v>258</v>
+      </c>
+      <c r="O105">
+        <v>42.744901982000002</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>112</v>
       </c>
@@ -22864,8 +23507,14 @@
       <c r="M106">
         <v>312.19893248699998</v>
       </c>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N106" t="s">
+        <v>259</v>
+      </c>
+      <c r="O106">
+        <v>19.556751817999999</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>113</v>
       </c>
@@ -22908,8 +23557,14 @@
       <c r="M107">
         <v>288.24064765700001</v>
       </c>
-    </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N107" t="s">
+        <v>259</v>
+      </c>
+      <c r="O107">
+        <v>20.949349660999999</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>114</v>
       </c>
@@ -22952,8 +23607,14 @@
       <c r="M108">
         <v>0.19384426900000001</v>
       </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N108" t="s">
+        <v>259</v>
+      </c>
+      <c r="O108">
+        <v>0.190186682</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>115</v>
       </c>
@@ -22996,8 +23657,14 @@
       <c r="M109">
         <v>0.16197946899999999</v>
       </c>
-    </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N109" t="s">
+        <v>259</v>
+      </c>
+      <c r="O109">
+        <v>0.158040387</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>116</v>
       </c>
@@ -23040,8 +23707,14 @@
       <c r="M110">
         <v>681.80943971900001</v>
       </c>
-    </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N110" t="s">
+        <v>259</v>
+      </c>
+      <c r="O110">
+        <v>12.561004586999999</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>117</v>
       </c>
@@ -23084,8 +23757,14 @@
       <c r="M111">
         <v>264.52458167600003</v>
       </c>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N111" t="s">
+        <v>259</v>
+      </c>
+      <c r="O111">
+        <v>20.920626780999999</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>118</v>
       </c>
@@ -23128,8 +23807,14 @@
       <c r="M112">
         <v>68.396624497999994</v>
       </c>
-    </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N112" t="s">
+        <v>261</v>
+      </c>
+      <c r="O112">
+        <v>17.392044086999999</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>119</v>
       </c>
@@ -23172,8 +23857,14 @@
       <c r="M113">
         <v>119.12664254400001</v>
       </c>
-    </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N113" t="s">
+        <v>261</v>
+      </c>
+      <c r="O113">
+        <v>17.898443388</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>120</v>
       </c>
@@ -23216,8 +23907,14 @@
       <c r="M114">
         <v>22.282320501000001</v>
       </c>
-    </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N114" t="s">
+        <v>261</v>
+      </c>
+      <c r="O114">
+        <v>19.056639103999998</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>121</v>
       </c>
@@ -23260,8 +23957,14 @@
       <c r="M115">
         <v>62.852743189000002</v>
       </c>
-    </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N115" t="s">
+        <v>261</v>
+      </c>
+      <c r="O115">
+        <v>16.689692017999999</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>122</v>
       </c>
@@ -23304,8 +24007,14 @@
       <c r="M116">
         <v>749.87047708700004</v>
       </c>
-    </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N116" t="s">
+        <v>261</v>
+      </c>
+      <c r="O116">
+        <v>18.955085491999998</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>123</v>
       </c>
@@ -23348,8 +24057,14 @@
       <c r="M117">
         <v>901.727393076</v>
       </c>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N117" t="s">
+        <v>261</v>
+      </c>
+      <c r="O117">
+        <v>18.310800082</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>124</v>
       </c>
@@ -23392,8 +24107,14 @@
       <c r="M118">
         <v>6.0374380810000003</v>
       </c>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N118" t="s">
+        <v>258</v>
+      </c>
+      <c r="O118">
+        <v>0.67848631000000004</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>125</v>
       </c>
@@ -23436,8 +24157,14 @@
       <c r="M119">
         <v>9.5843368089999998</v>
       </c>
-    </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N119" t="s">
+        <v>259</v>
+      </c>
+      <c r="O119">
+        <v>0.66767466499999995</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>126</v>
       </c>
@@ -23480,8 +24207,14 @@
       <c r="M120">
         <v>8.3666505010000005</v>
       </c>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N120" t="s">
+        <v>259</v>
+      </c>
+      <c r="O120">
+        <v>0.50250746000000002</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>127</v>
       </c>
@@ -23524,8 +24257,14 @@
       <c r="M121">
         <v>4.2081603750000003</v>
       </c>
-    </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N121" t="s">
+        <v>259</v>
+      </c>
+      <c r="O121">
+        <v>0.489757096</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>128</v>
       </c>
@@ -23568,8 +24307,14 @@
       <c r="M122">
         <v>8.2588015119999998</v>
       </c>
-    </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N122" t="s">
+        <v>258</v>
+      </c>
+      <c r="O122">
+        <v>0.64663804499999999</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>129</v>
       </c>
@@ -23612,8 +24357,14 @@
       <c r="M123">
         <v>2.234756285</v>
       </c>
-    </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N123" t="s">
+        <v>259</v>
+      </c>
+      <c r="O123">
+        <v>1.327142716</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>130</v>
       </c>
@@ -23656,8 +24407,14 @@
       <c r="M124">
         <v>126.841352896</v>
       </c>
-    </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N124" t="s">
+        <v>259</v>
+      </c>
+      <c r="O124">
+        <v>0.50352679899999997</v>
+      </c>
+    </row>
+    <row r="125" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>131</v>
       </c>
@@ -23700,8 +24457,14 @@
       <c r="M125">
         <v>3.37590557</v>
       </c>
-    </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N125" t="s">
+        <v>259</v>
+      </c>
+      <c r="O125">
+        <v>0.46161991499999999</v>
+      </c>
+    </row>
+    <row r="126" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>132</v>
       </c>
@@ -23744,8 +24507,14 @@
       <c r="M126">
         <v>2.219374111</v>
       </c>
-    </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N126" t="s">
+        <v>259</v>
+      </c>
+      <c r="O126">
+        <v>1.3252805299999999</v>
+      </c>
+    </row>
+    <row r="127" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>133</v>
       </c>
@@ -23788,8 +24557,14 @@
       <c r="M127">
         <v>0.73418394099999995</v>
       </c>
-    </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N127" t="s">
+        <v>258</v>
+      </c>
+      <c r="O127">
+        <v>0.178590621</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>134</v>
       </c>
@@ -23832,8 +24607,14 @@
       <c r="M128">
         <v>0.77841205099999999</v>
       </c>
-    </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N128" t="s">
+        <v>259</v>
+      </c>
+      <c r="O128">
+        <v>0.321617614</v>
+      </c>
+    </row>
+    <row r="129" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>135</v>
       </c>
@@ -23876,8 +24657,14 @@
       <c r="M129">
         <v>0.69441493300000001</v>
       </c>
-    </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N129" t="s">
+        <v>258</v>
+      </c>
+      <c r="O129">
+        <v>0.35028008500000002</v>
+      </c>
+    </row>
+    <row r="130" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>136</v>
       </c>
@@ -23920,8 +24707,14 @@
       <c r="M130">
         <v>0.95457138500000005</v>
       </c>
-    </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N130" t="s">
+        <v>259</v>
+      </c>
+      <c r="O130">
+        <v>0.33422856499999998</v>
+      </c>
+    </row>
+    <row r="131" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>137</v>
       </c>
@@ -23964,8 +24757,14 @@
       <c r="M131">
         <v>0.67042240600000003</v>
       </c>
-    </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N131" t="s">
+        <v>259</v>
+      </c>
+      <c r="O131">
+        <v>0.32889796399999999</v>
+      </c>
+    </row>
+    <row r="132" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>138</v>
       </c>
@@ -24008,8 +24807,14 @@
       <c r="M132">
         <v>2.227327898</v>
       </c>
-    </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N132" t="s">
+        <v>259</v>
+      </c>
+      <c r="O132">
+        <v>0.31513310700000002</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>139</v>
       </c>
@@ -24052,8 +24857,14 @@
       <c r="M133">
         <v>3.8963631400000001</v>
       </c>
-    </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N133" t="s">
+        <v>259</v>
+      </c>
+      <c r="O133">
+        <v>0.95982263599999995</v>
+      </c>
+    </row>
+    <row r="134" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>140</v>
       </c>
@@ -24096,8 +24907,14 @@
       <c r="M134">
         <v>2.471347593</v>
       </c>
-    </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N134" t="s">
+        <v>259</v>
+      </c>
+      <c r="O134">
+        <v>0.239026338</v>
+      </c>
+    </row>
+    <row r="135" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>141</v>
       </c>
@@ -24140,8 +24957,14 @@
       <c r="M135">
         <v>240.38835290700001</v>
       </c>
-    </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N135" t="s">
+        <v>259</v>
+      </c>
+      <c r="O135">
+        <v>1.3195639349999999</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>142</v>
       </c>
@@ -24184,8 +25007,14 @@
       <c r="M136">
         <v>483.20236474199999</v>
       </c>
-    </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N136" t="s">
+        <v>259</v>
+      </c>
+      <c r="O136">
+        <v>0.86266341300000005</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>143</v>
       </c>
@@ -24228,8 +25057,14 @@
       <c r="M137">
         <v>218.622913168</v>
       </c>
-    </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N137" t="s">
+        <v>259</v>
+      </c>
+      <c r="O137">
+        <v>1.534992514</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>144</v>
       </c>
@@ -24272,8 +25107,14 @@
       <c r="M138">
         <v>901.60462567900004</v>
       </c>
-    </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N138" t="s">
+        <v>259</v>
+      </c>
+      <c r="O138">
+        <v>1.0248982339999999</v>
+      </c>
+    </row>
+    <row r="139" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>145</v>
       </c>
@@ -24316,8 +25157,14 @@
       <c r="M139">
         <v>4.5328894550000003</v>
       </c>
-    </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N139" t="s">
+        <v>258</v>
+      </c>
+      <c r="O139">
+        <v>0.221830572</v>
+      </c>
+    </row>
+    <row r="140" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>146</v>
       </c>
@@ -24360,8 +25207,14 @@
       <c r="M140">
         <v>4.7089380409999997</v>
       </c>
-    </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N140" t="s">
+        <v>259</v>
+      </c>
+      <c r="O140">
+        <v>0.44631717100000001</v>
+      </c>
+    </row>
+    <row r="141" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>147</v>
       </c>
@@ -24404,8 +25257,14 @@
       <c r="M141">
         <v>1.998844163</v>
       </c>
-    </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N141" t="s">
+        <v>258</v>
+      </c>
+      <c r="O141">
+        <v>0.24257988599999999</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>148</v>
       </c>
@@ -24448,8 +25307,14 @@
       <c r="M142">
         <v>416.90210300699999</v>
       </c>
-    </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N142" t="s">
+        <v>259</v>
+      </c>
+      <c r="O142">
+        <v>0.60336353799999998</v>
+      </c>
+    </row>
+    <row r="143" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>149</v>
       </c>
@@ -24492,8 +25357,14 @@
       <c r="M143">
         <v>6.9754878000000006E-2</v>
       </c>
-    </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N143" t="s">
+        <v>259</v>
+      </c>
+      <c r="O143">
+        <v>7.0369256000000005E-2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>150</v>
       </c>
@@ -24536,8 +25407,14 @@
       <c r="M144">
         <v>901.72192235</v>
       </c>
-    </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N144" t="s">
+        <v>258</v>
+      </c>
+      <c r="O144">
+        <v>0.69071374699999999</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>151</v>
       </c>
@@ -24580,8 +25457,14 @@
       <c r="M145">
         <v>901.70730279999998</v>
       </c>
-    </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N145" t="s">
+        <v>259</v>
+      </c>
+      <c r="O145">
+        <v>1.0591393410000001</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>152</v>
       </c>
@@ -24624,8 +25507,14 @@
       <c r="M146">
         <v>901.71131255800003</v>
       </c>
-    </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N146" t="s">
+        <v>259</v>
+      </c>
+      <c r="O146">
+        <v>0.70905900099999997</v>
+      </c>
+    </row>
+    <row r="147" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>153</v>
       </c>
@@ -24668,8 +25557,14 @@
       <c r="M147">
         <v>901.71389984899997</v>
       </c>
-    </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N147" t="s">
+        <v>258</v>
+      </c>
+      <c r="O147">
+        <v>0.71991240099999998</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>154</v>
       </c>
@@ -24712,8 +25607,14 @@
       <c r="M148">
         <v>901.70956968600001</v>
       </c>
-    </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N148" t="s">
+        <v>258</v>
+      </c>
+      <c r="O148">
+        <v>0.91843636299999998</v>
+      </c>
+    </row>
+    <row r="149" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>155</v>
       </c>
@@ -24756,8 +25657,14 @@
       <c r="M149">
         <v>901.60518767999997</v>
       </c>
-    </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N149" t="s">
+        <v>258</v>
+      </c>
+      <c r="O149">
+        <v>1.367753789</v>
+      </c>
+    </row>
+    <row r="150" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>156</v>
       </c>
@@ -24800,8 +25707,14 @@
       <c r="M150">
         <v>901.72209818500005</v>
       </c>
-    </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N150" t="s">
+        <v>259</v>
+      </c>
+      <c r="O150">
+        <v>0.96197991100000002</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>157</v>
       </c>
@@ -24844,8 +25757,14 @@
       <c r="M151">
         <v>28.806528774</v>
       </c>
-    </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N151" t="s">
+        <v>259</v>
+      </c>
+      <c r="O151">
+        <v>29.010605904999998</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>158</v>
       </c>
@@ -24888,8 +25807,14 @@
       <c r="M152">
         <v>18.907693205000001</v>
       </c>
-    </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N152" t="s">
+        <v>259</v>
+      </c>
+      <c r="O152">
+        <v>18.968141493000001</v>
+      </c>
+    </row>
+    <row r="153" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>159</v>
       </c>
@@ -24932,8 +25857,14 @@
       <c r="M153">
         <v>3.7166006989999998</v>
       </c>
-    </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N153" t="s">
+        <v>259</v>
+      </c>
+      <c r="O153">
+        <v>1.0719999929999999</v>
+      </c>
+    </row>
+    <row r="154" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>160</v>
       </c>
@@ -24976,8 +25907,14 @@
       <c r="M154">
         <v>1.410813675</v>
       </c>
-    </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N154" t="s">
+        <v>259</v>
+      </c>
+      <c r="O154">
+        <v>1.0027159729999999</v>
+      </c>
+    </row>
+    <row r="155" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>161</v>
       </c>
@@ -25020,8 +25957,14 @@
       <c r="M155">
         <v>19.011272508000001</v>
       </c>
-    </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N155" t="s">
+        <v>259</v>
+      </c>
+      <c r="O155">
+        <v>19.198952959</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>162</v>
       </c>
@@ -25064,8 +26007,14 @@
       <c r="M156">
         <v>0.29795597400000001</v>
       </c>
-    </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N156" t="s">
+        <v>258</v>
+      </c>
+      <c r="O156">
+        <v>0.97965506099999999</v>
+      </c>
+    </row>
+    <row r="157" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>163</v>
       </c>
@@ -25108,8 +26057,14 @@
       <c r="M157">
         <v>1.154659076</v>
       </c>
-    </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N157" t="s">
+        <v>258</v>
+      </c>
+      <c r="O157">
+        <v>0.96330579500000002</v>
+      </c>
+    </row>
+    <row r="158" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>164</v>
       </c>
@@ -25152,8 +26107,14 @@
       <c r="M158">
         <v>2.7197133519999999</v>
       </c>
-    </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N158" t="s">
+        <v>259</v>
+      </c>
+      <c r="O158">
+        <v>0.93128535000000001</v>
+      </c>
+    </row>
+    <row r="159" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>165</v>
       </c>
@@ -25196,8 +26157,14 @@
       <c r="M159">
         <v>29.226698196000001</v>
       </c>
-    </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N159" t="s">
+        <v>258</v>
+      </c>
+      <c r="O159">
+        <v>28.856187294000001</v>
+      </c>
+    </row>
+    <row r="160" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>166</v>
       </c>
@@ -25240,8 +26207,14 @@
       <c r="M160">
         <v>49.710790842999998</v>
       </c>
-    </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N160" t="s">
+        <v>259</v>
+      </c>
+      <c r="O160">
+        <v>49.811337211000001</v>
+      </c>
+    </row>
+    <row r="161" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>167</v>
       </c>
@@ -25284,8 +26257,14 @@
       <c r="M161">
         <v>2.711702528</v>
       </c>
-    </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N161" t="s">
+        <v>259</v>
+      </c>
+      <c r="O161">
+        <v>0.94631692199999995</v>
+      </c>
+    </row>
+    <row r="162" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>168</v>
       </c>
@@ -25328,8 +26307,14 @@
       <c r="M162">
         <v>2.1233887400000002</v>
       </c>
-    </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N162" t="s">
+        <v>259</v>
+      </c>
+      <c r="O162">
+        <v>1.3262818000000001</v>
+      </c>
+    </row>
+    <row r="163" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>169</v>
       </c>
@@ -25372,8 +26357,14 @@
       <c r="M163">
         <v>28.714915801</v>
       </c>
-    </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N163" t="s">
+        <v>259</v>
+      </c>
+      <c r="O163">
+        <v>29.258674672000001</v>
+      </c>
+    </row>
+    <row r="164" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>170</v>
       </c>
@@ -25416,8 +26407,14 @@
       <c r="M164">
         <v>0.29394513</v>
       </c>
-    </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N164" t="s">
+        <v>258</v>
+      </c>
+      <c r="O164">
+        <v>0.97518547</v>
+      </c>
+    </row>
+    <row r="165" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>171</v>
       </c>
@@ -25460,8 +26457,14 @@
       <c r="M165">
         <v>3.3797854000000002E-2</v>
       </c>
-    </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N165" t="s">
+        <v>259</v>
+      </c>
+      <c r="O165">
+        <v>5.4594563999999998E-2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>172</v>
       </c>
@@ -25504,8 +26507,14 @@
       <c r="M166">
         <v>3.7815762000000003E-2</v>
       </c>
-    </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N166" t="s">
+        <v>258</v>
+      </c>
+      <c r="O166">
+        <v>5.8655194000000001E-2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>173</v>
       </c>
@@ -25548,8 +26557,14 @@
       <c r="M167">
         <v>3.3869877999999999E-2</v>
       </c>
-    </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N167" t="s">
+        <v>259</v>
+      </c>
+      <c r="O167">
+        <v>5.4705129999999998E-2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>174</v>
       </c>
@@ -25592,8 +26607,14 @@
       <c r="M168">
         <v>3.3795947E-2</v>
       </c>
-    </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N168" t="s">
+        <v>259</v>
+      </c>
+      <c r="O168">
+        <v>5.4454664E-2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>175</v>
       </c>
@@ -25636,8 +26657,14 @@
       <c r="M169">
         <v>3.7868341E-2</v>
       </c>
-    </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N169" t="s">
+        <v>258</v>
+      </c>
+      <c r="O169">
+        <v>5.4386715000000002E-2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>176</v>
       </c>
@@ -25680,8 +26707,14 @@
       <c r="M170">
         <v>3.7895854E-2</v>
       </c>
-    </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N170" t="s">
+        <v>258</v>
+      </c>
+      <c r="O170">
+        <v>5.4457564999999999E-2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>177</v>
       </c>
@@ -25724,8 +26757,14 @@
       <c r="M171">
         <v>4.6335029E-2</v>
       </c>
-    </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N171" t="s">
+        <v>258</v>
+      </c>
+      <c r="O171">
+        <v>6.6437288999999997E-2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>178</v>
       </c>
@@ -25768,8 +26807,14 @@
       <c r="M172">
         <v>3.4005318999999999E-2</v>
       </c>
-    </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N172" t="s">
+        <v>259</v>
+      </c>
+      <c r="O172">
+        <v>6.2907109000000003E-2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>179</v>
       </c>
@@ -25812,8 +26857,14 @@
       <c r="M173">
         <v>4.2295168000000001E-2</v>
       </c>
-    </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N173" t="s">
+        <v>259</v>
+      </c>
+      <c r="O173">
+        <v>6.3384983000000006E-2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>180</v>
       </c>
@@ -25856,8 +26907,14 @@
       <c r="M174">
         <v>901.84394919500005</v>
       </c>
-    </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N174" t="s">
+        <v>260</v>
+      </c>
+      <c r="O174">
+        <v>901.68339887000002</v>
+      </c>
+    </row>
+    <row r="175" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>181</v>
       </c>
@@ -25900,8 +26957,14 @@
       <c r="M175">
         <v>268.17617553500003</v>
       </c>
-    </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N175" t="s">
+        <v>260</v>
+      </c>
+      <c r="O175">
+        <v>901.68970168999999</v>
+      </c>
+    </row>
+    <row r="176" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>182</v>
       </c>
@@ -25944,8 +27007,14 @@
       <c r="M176">
         <v>261.95835160299998</v>
       </c>
-    </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N176" t="s">
+        <v>260</v>
+      </c>
+      <c r="O176">
+        <v>901.59228063700004</v>
+      </c>
+    </row>
+    <row r="177" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>183</v>
       </c>
@@ -25988,8 +27057,14 @@
       <c r="M177">
         <v>345.43369718500003</v>
       </c>
-    </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N177" t="s">
+        <v>260</v>
+      </c>
+      <c r="O177">
+        <v>901.68485048900004</v>
+      </c>
+    </row>
+    <row r="178" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>184</v>
       </c>
@@ -26032,8 +27107,14 @@
       <c r="M178">
         <v>209.84469724499999</v>
       </c>
-    </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N178" t="s">
+        <v>260</v>
+      </c>
+      <c r="O178">
+        <v>901.68788792600003</v>
+      </c>
+    </row>
+    <row r="179" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>185</v>
       </c>
@@ -26076,8 +27157,14 @@
       <c r="M179">
         <v>361.64644872700001</v>
       </c>
-    </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N179" t="s">
+        <v>260</v>
+      </c>
+      <c r="O179">
+        <v>901.68929959299999</v>
+      </c>
+    </row>
+    <row r="180" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>186</v>
       </c>
@@ -26120,8 +27207,14 @@
       <c r="M180">
         <v>423.08887849600001</v>
       </c>
-    </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N180" t="s">
+        <v>260</v>
+      </c>
+      <c r="O180">
+        <v>901.67795110199995</v>
+      </c>
+    </row>
+    <row r="181" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>187</v>
       </c>
@@ -26164,8 +27257,14 @@
       <c r="M181">
         <v>901.82741969400001</v>
       </c>
-    </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N181" t="s">
+        <v>260</v>
+      </c>
+      <c r="O181">
+        <v>901.68385272399996</v>
+      </c>
+    </row>
+    <row r="182" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>188</v>
       </c>
@@ -26208,8 +27307,14 @@
       <c r="M182">
         <v>331.86981630399998</v>
       </c>
-    </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N182" t="s">
+        <v>260</v>
+      </c>
+      <c r="O182">
+        <v>901.58936132500003</v>
+      </c>
+    </row>
+    <row r="183" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>189</v>
       </c>
@@ -26252,8 +27357,14 @@
       <c r="M183">
         <v>209.080923345</v>
       </c>
-    </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N183" t="s">
+        <v>260</v>
+      </c>
+      <c r="O183">
+        <v>901.68519611900001</v>
+      </c>
+    </row>
+    <row r="184" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>190</v>
       </c>
@@ -26296,8 +27407,14 @@
       <c r="M184">
         <v>901.821976683</v>
       </c>
-    </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N184" t="s">
+        <v>260</v>
+      </c>
+      <c r="O184">
+        <v>901.69205003800005</v>
+      </c>
+    </row>
+    <row r="185" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>191</v>
       </c>
@@ -26340,8 +27457,14 @@
       <c r="M185">
         <v>901.90221757999996</v>
       </c>
-    </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N185" t="s">
+        <v>260</v>
+      </c>
+      <c r="O185">
+        <v>901.691398123</v>
+      </c>
+    </row>
+    <row r="186" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>192</v>
       </c>
@@ -26384,8 +27507,14 @@
       <c r="M186">
         <v>901.65419067799996</v>
       </c>
-    </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N186" t="s">
+        <v>260</v>
+      </c>
+      <c r="O186">
+        <v>901.68360467599996</v>
+      </c>
+    </row>
+    <row r="187" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>193</v>
       </c>
@@ -26428,8 +27557,14 @@
       <c r="M187">
         <v>901.78661057600004</v>
       </c>
-    </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N187" t="s">
+        <v>260</v>
+      </c>
+      <c r="O187">
+        <v>901.67297041100005</v>
+      </c>
+    </row>
+    <row r="188" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>194</v>
       </c>
@@ -26472,8 +27607,14 @@
       <c r="M188">
         <v>901.68789050199996</v>
       </c>
-    </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N188" t="s">
+        <v>260</v>
+      </c>
+      <c r="O188">
+        <v>901.58772184899999</v>
+      </c>
+    </row>
+    <row r="189" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>195</v>
       </c>
@@ -26516,8 +27657,14 @@
       <c r="M189">
         <v>462.71311323999998</v>
       </c>
-    </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N189" t="s">
+        <v>260</v>
+      </c>
+      <c r="O189">
+        <v>901.68377849700005</v>
+      </c>
+    </row>
+    <row r="190" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>196</v>
       </c>
@@ -26560,8 +27707,14 @@
       <c r="M190">
         <v>374.06800933400001</v>
       </c>
-    </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N190" t="s">
+        <v>258</v>
+      </c>
+      <c r="O190">
+        <v>16.245493080999999</v>
+      </c>
+    </row>
+    <row r="191" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>197</v>
       </c>
@@ -26604,8 +27757,14 @@
       <c r="M191">
         <v>376.31528081800002</v>
       </c>
-    </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N191" t="s">
+        <v>259</v>
+      </c>
+      <c r="O191">
+        <v>44.394362800000003</v>
+      </c>
+    </row>
+    <row r="192" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>198</v>
       </c>
@@ -26648,8 +27807,14 @@
       <c r="M192">
         <v>377.71510604000002</v>
       </c>
-    </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N192" t="s">
+        <v>259</v>
+      </c>
+      <c r="O192">
+        <v>9.1604559830000003</v>
+      </c>
+    </row>
+    <row r="193" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>199</v>
       </c>
@@ -26692,8 +27857,14 @@
       <c r="M193">
         <v>377.81247649099998</v>
       </c>
-    </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N193" t="s">
+        <v>259</v>
+      </c>
+      <c r="O193">
+        <v>13.995950651999999</v>
+      </c>
+    </row>
+    <row r="194" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>200</v>
       </c>
@@ -26736,8 +27907,14 @@
       <c r="M194">
         <v>375.631682012</v>
       </c>
-    </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N194" t="s">
+        <v>259</v>
+      </c>
+      <c r="O194">
+        <v>32.645811352999999</v>
+      </c>
+    </row>
+    <row r="195" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>201</v>
       </c>
@@ -26780,8 +27957,14 @@
       <c r="M195">
         <v>374.189628981</v>
       </c>
-    </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N195" t="s">
+        <v>259</v>
+      </c>
+      <c r="O195">
+        <v>58.809339475000002</v>
+      </c>
+    </row>
+    <row r="196" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>202</v>
       </c>
@@ -26824,8 +28007,14 @@
       <c r="M196">
         <v>375.76876824499999</v>
       </c>
-    </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N196" t="s">
+        <v>259</v>
+      </c>
+      <c r="O196">
+        <v>26.217260850999999</v>
+      </c>
+    </row>
+    <row r="197" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>203</v>
       </c>
@@ -26868,8 +28057,14 @@
       <c r="M197">
         <v>377.18767766799999</v>
       </c>
-    </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N197" t="s">
+        <v>259</v>
+      </c>
+      <c r="O197">
+        <v>46.047832022000001</v>
+      </c>
+    </row>
+    <row r="198" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>204</v>
       </c>
@@ -26912,8 +28107,14 @@
       <c r="M198">
         <v>377.79432568999999</v>
       </c>
-    </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N198" t="s">
+        <v>260</v>
+      </c>
+      <c r="O198">
+        <v>901.68922245199997</v>
+      </c>
+    </row>
+    <row r="199" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>205</v>
       </c>
@@ -26956,8 +28157,14 @@
       <c r="M199">
         <v>378.33288976599999</v>
       </c>
-    </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N199" t="s">
+        <v>258</v>
+      </c>
+      <c r="O199">
+        <v>51.271604052999997</v>
+      </c>
+    </row>
+    <row r="200" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>206</v>
       </c>
@@ -27000,8 +28207,14 @@
       <c r="M200">
         <v>377.58575077299997</v>
       </c>
-    </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N200" t="s">
+        <v>260</v>
+      </c>
+      <c r="O200">
+        <v>901.69347850400004</v>
+      </c>
+    </row>
+    <row r="201" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>207</v>
       </c>
@@ -27044,8 +28257,14 @@
       <c r="M201">
         <v>374.63396084599998</v>
       </c>
-    </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N201" t="s">
+        <v>259</v>
+      </c>
+      <c r="O201">
+        <v>586.47599216900005</v>
+      </c>
+    </row>
+    <row r="202" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>208</v>
       </c>
@@ -27088,8 +28307,14 @@
       <c r="M202">
         <v>371.74990883800001</v>
       </c>
-    </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N202" t="s">
+        <v>259</v>
+      </c>
+      <c r="O202">
+        <v>104.410285847</v>
+      </c>
+    </row>
+    <row r="203" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>209</v>
       </c>
@@ -27132,8 +28357,14 @@
       <c r="M203">
         <v>375.531094338</v>
       </c>
-    </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N203" t="s">
+        <v>259</v>
+      </c>
+      <c r="O203">
+        <v>784.65837651000004</v>
+      </c>
+    </row>
+    <row r="204" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>210</v>
       </c>
@@ -27176,8 +28407,14 @@
       <c r="M204">
         <v>379.12666924899997</v>
       </c>
-    </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N204" t="s">
+        <v>260</v>
+      </c>
+      <c r="O204">
+        <v>901.678012954</v>
+      </c>
+    </row>
+    <row r="205" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>211</v>
       </c>
@@ -27220,8 +28457,14 @@
       <c r="M205">
         <v>901.92117202400004</v>
       </c>
-    </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N205" t="s">
+        <v>258</v>
+      </c>
+      <c r="O205">
+        <v>9.7887999210000007</v>
+      </c>
+    </row>
+    <row r="206" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>212</v>
       </c>
@@ -27264,8 +28507,14 @@
       <c r="M206">
         <v>901.91152725899997</v>
       </c>
-    </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N206" t="s">
+        <v>259</v>
+      </c>
+      <c r="O206">
+        <v>21.253559467999999</v>
+      </c>
+    </row>
+    <row r="207" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>213</v>
       </c>
@@ -27308,8 +28557,14 @@
       <c r="M207">
         <v>901.93081161999999</v>
       </c>
-    </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N207" t="s">
+        <v>259</v>
+      </c>
+      <c r="O207">
+        <v>7.787452665</v>
+      </c>
+    </row>
+    <row r="208" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>214</v>
       </c>
@@ -27352,8 +28607,14 @@
       <c r="M208">
         <v>901.94422756799997</v>
       </c>
-    </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N208" t="s">
+        <v>259</v>
+      </c>
+      <c r="O208">
+        <v>26.713495036000001</v>
+      </c>
+    </row>
+    <row r="209" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>215</v>
       </c>
@@ -27396,8 +28657,14 @@
       <c r="M209">
         <v>901.97942791100002</v>
       </c>
-    </row>
-    <row r="210" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N209" t="s">
+        <v>259</v>
+      </c>
+      <c r="O209">
+        <v>25.344532386000001</v>
+      </c>
+    </row>
+    <row r="210" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>216</v>
       </c>
@@ -27440,8 +28707,14 @@
       <c r="M210">
         <v>901.86674174899997</v>
       </c>
-    </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N210" t="s">
+        <v>259</v>
+      </c>
+      <c r="O210">
+        <v>76.154035636000003</v>
+      </c>
+    </row>
+    <row r="211" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>217</v>
       </c>
@@ -27484,8 +28757,14 @@
       <c r="M211">
         <v>901.91676658599999</v>
       </c>
-    </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N211" t="s">
+        <v>259</v>
+      </c>
+      <c r="O211">
+        <v>6.6547002060000002</v>
+      </c>
+    </row>
+    <row r="212" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>218</v>
       </c>
@@ -27528,8 +28807,14 @@
       <c r="M212">
         <v>901.90377795400002</v>
       </c>
-    </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N212" t="s">
+        <v>259</v>
+      </c>
+      <c r="O212">
+        <v>55.771123819000003</v>
+      </c>
+    </row>
+    <row r="213" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>219</v>
       </c>
@@ -27572,8 +28857,14 @@
       <c r="M213">
         <v>901.922943465</v>
       </c>
-    </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N213" t="s">
+        <v>259</v>
+      </c>
+      <c r="O213">
+        <v>29.375474236999999</v>
+      </c>
+    </row>
+    <row r="214" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>220</v>
       </c>
@@ -27616,8 +28907,14 @@
       <c r="M214">
         <v>901.92663570499997</v>
       </c>
-    </row>
-    <row r="215" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N214" t="s">
+        <v>259</v>
+      </c>
+      <c r="O214">
+        <v>11.646405788999999</v>
+      </c>
+    </row>
+    <row r="215" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>221</v>
       </c>
@@ -27660,8 +28957,14 @@
       <c r="M215">
         <v>901.93464306500005</v>
       </c>
-    </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N215" t="s">
+        <v>259</v>
+      </c>
+      <c r="O215">
+        <v>31.817285194</v>
+      </c>
+    </row>
+    <row r="216" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>222</v>
       </c>
@@ -27704,8 +29007,14 @@
       <c r="M216">
         <v>901.83585109000001</v>
       </c>
-    </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N216" t="s">
+        <v>259</v>
+      </c>
+      <c r="O216">
+        <v>101.49295087100001</v>
+      </c>
+    </row>
+    <row r="217" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>223</v>
       </c>
@@ -27748,8 +29057,14 @@
       <c r="M217">
         <v>901.90973408499997</v>
       </c>
-    </row>
-    <row r="218" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N217" t="s">
+        <v>259</v>
+      </c>
+      <c r="O217">
+        <v>85.596985485999994</v>
+      </c>
+    </row>
+    <row r="218" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>224</v>
       </c>
@@ -27792,8 +29107,14 @@
       <c r="M218">
         <v>901.91082040000003</v>
       </c>
-    </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N218" t="s">
+        <v>259</v>
+      </c>
+      <c r="O218">
+        <v>151.53297589100001</v>
+      </c>
+    </row>
+    <row r="219" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>225</v>
       </c>
@@ -27836,8 +29157,14 @@
       <c r="M219">
         <v>901.90571349100003</v>
       </c>
-    </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N219" t="s">
+        <v>259</v>
+      </c>
+      <c r="O219">
+        <v>12.550783701</v>
+      </c>
+    </row>
+    <row r="220" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>226</v>
       </c>
@@ -27880,8 +29207,14 @@
       <c r="M220">
         <v>901.92103414999997</v>
       </c>
-    </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N220" t="s">
+        <v>259</v>
+      </c>
+      <c r="O220">
+        <v>158.56752614499999</v>
+      </c>
+    </row>
+    <row r="221" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>227</v>
       </c>
@@ -27924,8 +29257,14 @@
       <c r="M221">
         <v>901.93062413999996</v>
       </c>
-    </row>
-    <row r="222" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N221" t="s">
+        <v>259</v>
+      </c>
+      <c r="O221">
+        <v>23.539143887000002</v>
+      </c>
+    </row>
+    <row r="222" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>228</v>
       </c>
@@ -27968,8 +29307,14 @@
       <c r="M222">
         <v>901.85482829800003</v>
       </c>
-    </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N222" t="s">
+        <v>259</v>
+      </c>
+      <c r="O222">
+        <v>29.891773778000001</v>
+      </c>
+    </row>
+    <row r="223" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>229</v>
       </c>
@@ -28012,8 +29357,14 @@
       <c r="M223">
         <v>901.90781900599995</v>
       </c>
-    </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N223" t="s">
+        <v>259</v>
+      </c>
+      <c r="O223">
+        <v>34.335069304000001</v>
+      </c>
+    </row>
+    <row r="224" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>230</v>
       </c>
@@ -28056,8 +29407,14 @@
       <c r="M224">
         <v>901.92949698300004</v>
       </c>
-    </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N224" t="s">
+        <v>259</v>
+      </c>
+      <c r="O224">
+        <v>11.650372427000001</v>
+      </c>
+    </row>
+    <row r="225" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>231</v>
       </c>
@@ -28100,8 +29457,14 @@
       <c r="M225">
         <v>289.82711357099998</v>
       </c>
-    </row>
-    <row r="226" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N225" t="s">
+        <v>259</v>
+      </c>
+      <c r="O225">
+        <v>3.0400152560000002</v>
+      </c>
+    </row>
+    <row r="226" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>232</v>
       </c>
@@ -28144,8 +29507,14 @@
       <c r="M226">
         <v>261.64033683299999</v>
       </c>
-    </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N226" t="s">
+        <v>259</v>
+      </c>
+      <c r="O226">
+        <v>1.7150334</v>
+      </c>
+    </row>
+    <row r="227" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>233</v>
       </c>
@@ -28188,8 +29557,14 @@
       <c r="M227">
         <v>288.73173312500001</v>
       </c>
-    </row>
-    <row r="228" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N227" t="s">
+        <v>259</v>
+      </c>
+      <c r="O227">
+        <v>1.7283370849999999</v>
+      </c>
+    </row>
+    <row r="228" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>234</v>
       </c>
@@ -28232,8 +29607,14 @@
       <c r="M228">
         <v>290.01823381899999</v>
       </c>
-    </row>
-    <row r="229" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N228" t="s">
+        <v>259</v>
+      </c>
+      <c r="O228">
+        <v>3.6488472729999999</v>
+      </c>
+    </row>
+    <row r="229" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>235</v>
       </c>
@@ -28276,8 +29657,14 @@
       <c r="M229">
         <v>285.29137780999997</v>
       </c>
-    </row>
-    <row r="230" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N229" t="s">
+        <v>259</v>
+      </c>
+      <c r="O229">
+        <v>2.663697124</v>
+      </c>
+    </row>
+    <row r="230" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>236</v>
       </c>
@@ -28320,8 +29707,14 @@
       <c r="M230">
         <v>319.41944276800001</v>
       </c>
-    </row>
-    <row r="231" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N230" t="s">
+        <v>259</v>
+      </c>
+      <c r="O230">
+        <v>1.4868983010000001</v>
+      </c>
+    </row>
+    <row r="231" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>237</v>
       </c>
@@ -28364,8 +29757,14 @@
       <c r="M231">
         <v>288.70854226099999</v>
       </c>
-    </row>
-    <row r="232" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N231" t="s">
+        <v>258</v>
+      </c>
+      <c r="O231">
+        <v>2.4435705749999999</v>
+      </c>
+    </row>
+    <row r="232" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>238</v>
       </c>
@@ -28408,8 +29807,14 @@
       <c r="M232">
         <v>286.97308317699998</v>
       </c>
-    </row>
-    <row r="233" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N232" t="s">
+        <v>259</v>
+      </c>
+      <c r="O232">
+        <v>11.230117954000001</v>
+      </c>
+    </row>
+    <row r="233" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>239</v>
       </c>
@@ -28452,8 +29857,14 @@
       <c r="M233">
         <v>289.080580467</v>
       </c>
-    </row>
-    <row r="234" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N233" t="s">
+        <v>259</v>
+      </c>
+      <c r="O233">
+        <v>1.7871180630000001</v>
+      </c>
+    </row>
+    <row r="234" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>240</v>
       </c>
@@ -28496,8 +29907,14 @@
       <c r="M234">
         <v>289.05284258699999</v>
       </c>
-    </row>
-    <row r="235" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N234" t="s">
+        <v>258</v>
+      </c>
+      <c r="O234">
+        <v>2.371633025</v>
+      </c>
+    </row>
+    <row r="235" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>241</v>
       </c>
@@ -28540,8 +29957,14 @@
       <c r="M235">
         <v>287.98360920900001</v>
       </c>
-    </row>
-    <row r="236" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N235" t="s">
+        <v>259</v>
+      </c>
+      <c r="O235">
+        <v>2.155372549</v>
+      </c>
+    </row>
+    <row r="236" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>242</v>
       </c>
@@ -28584,8 +30007,14 @@
       <c r="M236">
         <v>289.84519299999999</v>
       </c>
-    </row>
-    <row r="237" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N236" t="s">
+        <v>259</v>
+      </c>
+      <c r="O236">
+        <v>4.2381726889999998</v>
+      </c>
+    </row>
+    <row r="237" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>243</v>
       </c>
@@ -28628,8 +30057,14 @@
       <c r="M237">
         <v>288.87610143400002</v>
       </c>
-    </row>
-    <row r="238" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N237" t="s">
+        <v>259</v>
+      </c>
+      <c r="O237">
+        <v>3.8966328130000001</v>
+      </c>
+    </row>
+    <row r="238" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>244</v>
       </c>
@@ -28672,8 +30107,14 @@
       <c r="M238">
         <v>290.936869452</v>
       </c>
-    </row>
-    <row r="239" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N238" t="s">
+        <v>259</v>
+      </c>
+      <c r="O238">
+        <v>2.3036372059999999</v>
+      </c>
+    </row>
+    <row r="239" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>245</v>
       </c>
@@ -28716,8 +30157,14 @@
       <c r="M239">
         <v>428.650032603</v>
       </c>
-    </row>
-    <row r="240" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N239" t="s">
+        <v>258</v>
+      </c>
+      <c r="O239">
+        <v>19.243596621999998</v>
+      </c>
+    </row>
+    <row r="240" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>246</v>
       </c>
@@ -28760,8 +30207,14 @@
       <c r="M240">
         <v>426.40971004800002</v>
       </c>
-    </row>
-    <row r="241" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N240" t="s">
+        <v>259</v>
+      </c>
+      <c r="O240">
+        <v>10.409617182</v>
+      </c>
+    </row>
+    <row r="241" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>247</v>
       </c>
@@ -28804,8 +30257,14 @@
       <c r="M241">
         <v>435.57989258100002</v>
       </c>
-    </row>
-    <row r="242" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N241" t="s">
+        <v>259</v>
+      </c>
+      <c r="O241">
+        <v>8.3960524329999995</v>
+      </c>
+    </row>
+    <row r="242" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>248</v>
       </c>
@@ -28848,8 +30307,14 @@
       <c r="M242">
         <v>427.64882749999998</v>
       </c>
-    </row>
-    <row r="243" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N242" t="s">
+        <v>259</v>
+      </c>
+      <c r="O242">
+        <v>8.2756081469999998</v>
+      </c>
+    </row>
+    <row r="243" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>249</v>
       </c>
@@ -28892,8 +30357,14 @@
       <c r="M243">
         <v>430.58283936700002</v>
       </c>
-    </row>
-    <row r="244" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N243" t="s">
+        <v>259</v>
+      </c>
+      <c r="O243">
+        <v>6.7104868069999997</v>
+      </c>
+    </row>
+    <row r="244" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>250</v>
       </c>
@@ -28936,8 +30407,14 @@
       <c r="M244">
         <v>433.05533016999999</v>
       </c>
-    </row>
-    <row r="245" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N244" t="s">
+        <v>259</v>
+      </c>
+      <c r="O244">
+        <v>5.1974418260000004</v>
+      </c>
+    </row>
+    <row r="245" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>251</v>
       </c>
@@ -28980,8 +30457,14 @@
       <c r="M245">
         <v>394.80382305000001</v>
       </c>
-    </row>
-    <row r="246" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N245" t="s">
+        <v>259</v>
+      </c>
+      <c r="O245">
+        <v>12.845981845000001</v>
+      </c>
+    </row>
+    <row r="246" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>252</v>
       </c>
@@ -29024,8 +30507,14 @@
       <c r="M246">
         <v>412.05375456199999</v>
       </c>
-    </row>
-    <row r="247" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N246" t="s">
+        <v>259</v>
+      </c>
+      <c r="O246">
+        <v>25.06044868</v>
+      </c>
+    </row>
+    <row r="247" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>253</v>
       </c>
@@ -29068,8 +30557,14 @@
       <c r="M247">
         <v>413.80258595700002</v>
       </c>
-    </row>
-    <row r="248" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N247" t="s">
+        <v>259</v>
+      </c>
+      <c r="O247">
+        <v>25.868731637</v>
+      </c>
+    </row>
+    <row r="248" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>254</v>
       </c>
@@ -29112,8 +30607,14 @@
       <c r="M248">
         <v>80.725753695999998</v>
       </c>
-    </row>
-    <row r="249" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N248" t="s">
+        <v>261</v>
+      </c>
+      <c r="O248">
+        <v>122.834903458</v>
+      </c>
+    </row>
+    <row r="249" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>255</v>
       </c>
@@ -29156,24 +30657,30 @@
       <c r="M249">
         <v>61.576339271999998</v>
       </c>
-    </row>
-    <row r="251" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N249" t="s">
+        <v>261</v>
+      </c>
+      <c r="O249">
+        <v>102.914173507</v>
+      </c>
+    </row>
+    <row r="251" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>275</v>
       </c>
-      <c r="B251">
+      <c r="B251" s="3">
         <f>COUNTIF(B4:B249,"sat") + COUNTIF(B4:B249,"unsat")</f>
         <v>27</v>
       </c>
-      <c r="D251">
+      <c r="D251" s="3">
         <f>COUNTIF(D4:D249,"sat") + COUNTIF(D4:D249,"unsat")</f>
         <v>43</v>
       </c>
-      <c r="F251">
+      <c r="F251" s="3">
         <f>COUNTIF(F4:F249,"sat") + COUNTIF(F4:F249,"unsat")</f>
         <v>139</v>
       </c>
-      <c r="H251">
+      <c r="H251" s="3">
         <f>COUNTIF(H4:H249,"sat") + COUNTIF(H4:H249,"unsat")</f>
         <v>111</v>
       </c>
@@ -29185,22 +30692,26 @@
         <f>COUNTIF(L4:L249,"sat") + COUNTIF(L4:L249,"unsat")</f>
         <v>72</v>
       </c>
-    </row>
-    <row r="252" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N251" s="3">
+        <f>COUNTIF(N4:N249,"sat") + COUNTIF(N4:N249,"unsat")</f>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="252" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>277</v>
       </c>
-      <c r="B252">
+      <c r="B252" s="3">
         <v>1</v>
       </c>
-      <c r="D252">
+      <c r="D252" s="3">
         <v>0</v>
       </c>
-      <c r="F252">
-        <v>22</v>
-      </c>
-      <c r="H252">
-        <v>9</v>
+      <c r="F252" s="3">
+        <v>5</v>
+      </c>
+      <c r="H252" s="3">
+        <v>1</v>
       </c>
       <c r="J252">
         <v>13</v>
@@ -29208,9 +30719,12 @@
       <c r="L252">
         <v>7</v>
       </c>
+      <c r="N252" s="3">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M252" xr:uid="{35486B71-12BE-2349-B57A-22BC9F8DFAFE}"/>
+  <autoFilter ref="A1:O249" xr:uid="{A71FF0FB-C798-074B-BAB4-A06B51F78A39}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>